<commit_message>
updated logit for asking and max_dropdown tolerance ranges
</commit_message>
<xml_diff>
--- a/Complete-List-of-iShares-ETFs-Traded-on-Toronto-Stock-Exchange-Jan-18-2025.xlsx
+++ b/Complete-List-of-iShares-ETFs-Traded-on-Toronto-Stock-Exchange-Jan-18-2025.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariadruker/Documents/Northeastern/5800/Final_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8FDA04-56B9-1247-8779-3B5920FBD25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3754065E-E644-DA49-B0D7-F1587E310163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="500" windowWidth="18460" windowHeight="16100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="500" windowWidth="25200" windowHeight="16100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -47,16 +49,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="485">
   <si>
     <t>Ticker</t>
   </si>
@@ -1037,6 +1053,480 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>SVR.TO</t>
+  </si>
+  <si>
+    <t>CGL.TO</t>
+  </si>
+  <si>
+    <t>XMV.TO</t>
+  </si>
+  <si>
+    <t>XMI.TO</t>
+  </si>
+  <si>
+    <t>XML.TO</t>
+  </si>
+  <si>
+    <t>XIN.TO</t>
+  </si>
+  <si>
+    <t>XMS.TO</t>
+  </si>
+  <si>
+    <t>XMY.TO</t>
+  </si>
+  <si>
+    <t>XEM.TO</t>
+  </si>
+  <si>
+    <t>XMM.TO</t>
+  </si>
+  <si>
+    <t>XEC.TO</t>
+  </si>
+  <si>
+    <t>XUS.TO</t>
+  </si>
+  <si>
+    <t>XEF.TO</t>
+  </si>
+  <si>
+    <t>XMH.TO</t>
+  </si>
+  <si>
+    <t>XMC.TO</t>
+  </si>
+  <si>
+    <t>XDIV.TO</t>
+  </si>
+  <si>
+    <t>XMU.TO</t>
+  </si>
+  <si>
+    <t>XQQ.TO</t>
+  </si>
+  <si>
+    <t>XWD.TO</t>
+  </si>
+  <si>
+    <t>XDUH.TO</t>
+  </si>
+  <si>
+    <t>XDG.TO</t>
+  </si>
+  <si>
+    <t>XSU.TO</t>
+  </si>
+  <si>
+    <t>XDU.TO</t>
+  </si>
+  <si>
+    <t>XSUS.TO</t>
+  </si>
+  <si>
+    <t>XSEA.TO</t>
+  </si>
+  <si>
+    <t>XDGH.TO</t>
+  </si>
+  <si>
+    <t>XESG.TO</t>
+  </si>
+  <si>
+    <t>XGI.TO</t>
+  </si>
+  <si>
+    <t>XCD.TO</t>
+  </si>
+  <si>
+    <t>XSEM.TO</t>
+  </si>
+  <si>
+    <t>XSP.TO</t>
+  </si>
+  <si>
+    <t>CWO.TO</t>
+  </si>
+  <si>
+    <t>CRQ.TO</t>
+  </si>
+  <si>
+    <t>XID.TO</t>
+  </si>
+  <si>
+    <t>XCH.TO</t>
+  </si>
+  <si>
+    <t>XEMC.TO</t>
+  </si>
+  <si>
+    <t>XHC.TO</t>
+  </si>
+  <si>
+    <t>XDRV.TO</t>
+  </si>
+  <si>
+    <t>CWW.TO</t>
+  </si>
+  <si>
+    <t>XCV.TO</t>
+  </si>
+  <si>
+    <t>XCG.TO</t>
+  </si>
+  <si>
+    <t>XUSR.TO</t>
+  </si>
+  <si>
+    <t>XDV.TO</t>
+  </si>
+  <si>
+    <t>XDSR.TO</t>
+  </si>
+  <si>
+    <t>XEU.TO</t>
+  </si>
+  <si>
+    <t>CEW.TO</t>
+  </si>
+  <si>
+    <t>XEH.TO</t>
+  </si>
+  <si>
+    <t>XUU.TO</t>
+  </si>
+  <si>
+    <t>COW.TO</t>
+  </si>
+  <si>
+    <t>CIF.TO</t>
+  </si>
+  <si>
+    <t>CYH.TO</t>
+  </si>
+  <si>
+    <t>XDNA.TO</t>
+  </si>
+  <si>
+    <t>XCLN.TO</t>
+  </si>
+  <si>
+    <t>XQQU.TO</t>
+  </si>
+  <si>
+    <t>XEXP.TO</t>
+  </si>
+  <si>
+    <t>XAW.TO</t>
+  </si>
+  <si>
+    <t>XHAK.TO</t>
+  </si>
+  <si>
+    <t>XETM.TO</t>
+  </si>
+  <si>
+    <t>XCHP.TO</t>
+  </si>
+  <si>
+    <t>CIE.TO</t>
+  </si>
+  <si>
+    <t>XUSF.TO</t>
+  </si>
+  <si>
+    <t>XAD.TO</t>
+  </si>
+  <si>
+    <t>XEN.TO</t>
+  </si>
+  <si>
+    <t>CUD.TO</t>
+  </si>
+  <si>
+    <t>CDZ.TO</t>
+  </si>
+  <si>
+    <t>XQLT.TO</t>
+  </si>
+  <si>
+    <t>XIU.TO</t>
+  </si>
+  <si>
+    <t>CJP.TO</t>
+  </si>
+  <si>
+    <t>XEG.TO</t>
+  </si>
+  <si>
+    <t>XST.TO</t>
+  </si>
+  <si>
+    <t>XIC.TO</t>
+  </si>
+  <si>
+    <t>CPD.TO</t>
+  </si>
+  <si>
+    <t>XSMC.TO</t>
+  </si>
+  <si>
+    <t>XMA.TO</t>
+  </si>
+  <si>
+    <t>XUSC.TO</t>
+  </si>
+  <si>
+    <t>XSMH.TO</t>
+  </si>
+  <si>
+    <t>XFH.TO</t>
+  </si>
+  <si>
+    <t>XIT.TO</t>
+  </si>
+  <si>
+    <t>XFN.TO</t>
+  </si>
+  <si>
+    <t>XMTM.TO</t>
+  </si>
+  <si>
+    <t>XBM.TO</t>
+  </si>
+  <si>
+    <t>XEI.TO</t>
+  </si>
+  <si>
+    <t>XVLU.TO</t>
+  </si>
+  <si>
+    <t>XMD.TO</t>
+  </si>
+  <si>
+    <t>XUT.TO</t>
+  </si>
+  <si>
+    <t>XCSR.TO</t>
+  </si>
+  <si>
+    <t>XPF.TO</t>
+  </si>
+  <si>
+    <t>XHU.TO</t>
+  </si>
+  <si>
+    <t>XGD.TO</t>
+  </si>
+  <si>
+    <t>XSPC.TO</t>
+  </si>
+  <si>
+    <t>XUH.TO</t>
+  </si>
+  <si>
+    <t>XCS.TO</t>
+  </si>
+  <si>
+    <t>XHD.TO</t>
+  </si>
+  <si>
+    <t>CLU.TO</t>
+  </si>
+  <si>
+    <t>XMW.TO</t>
+  </si>
+  <si>
+    <t>XSC.TO</t>
+  </si>
+  <si>
+    <t>XSE.TO</t>
+  </si>
+  <si>
+    <t>CMR.TO</t>
+  </si>
+  <si>
+    <t>CLG.TO</t>
+  </si>
+  <si>
+    <t>CBH.TO</t>
+  </si>
+  <si>
+    <t>CLF.TO</t>
+  </si>
+  <si>
+    <t>CBO.TO</t>
+  </si>
+  <si>
+    <t>CVD.TO</t>
+  </si>
+  <si>
+    <t>XQB.TO</t>
+  </si>
+  <si>
+    <t>XAGG.TO</t>
+  </si>
+  <si>
+    <t>XCBG.TO</t>
+  </si>
+  <si>
+    <t>XSHG.TO</t>
+  </si>
+  <si>
+    <t>XAGH.TO</t>
+  </si>
+  <si>
+    <t>XSTB.TO</t>
+  </si>
+  <si>
+    <t>XFLB.TO</t>
+  </si>
+  <si>
+    <t>XFLI.TO</t>
+  </si>
+  <si>
+    <t>XFLX.TO</t>
+  </si>
+  <si>
+    <t>XSAB.TO</t>
+  </si>
+  <si>
+    <t>XTLH.TO</t>
+  </si>
+  <si>
+    <t>XTLT.TO</t>
+  </si>
+  <si>
+    <t>XFR.TO</t>
+  </si>
+  <si>
+    <t>XGB.TO</t>
+  </si>
+  <si>
+    <t>XCB.TO</t>
+  </si>
+  <si>
+    <t>XSB.TO</t>
+  </si>
+  <si>
+    <t>XSI.TO</t>
+  </si>
+  <si>
+    <t>XRB.TO</t>
+  </si>
+  <si>
+    <t>XLB.TO</t>
+  </si>
+  <si>
+    <t>XHB.TO</t>
+  </si>
+  <si>
+    <t>XBB.TO</t>
+  </si>
+  <si>
+    <t>XSH.TO</t>
+  </si>
+  <si>
+    <t>XSTH.TO</t>
+  </si>
+  <si>
+    <t>XSTP.TO</t>
+  </si>
+  <si>
+    <t>XCBU.TO</t>
+  </si>
+  <si>
+    <t>XIGS.TO</t>
+  </si>
+  <si>
+    <t>XSHU.TO</t>
+  </si>
+  <si>
+    <t>XEB.TO</t>
+  </si>
+  <si>
+    <t>XIG.TO</t>
+  </si>
+  <si>
+    <t>XHY.TO</t>
+  </si>
+  <si>
+    <t>GCNS.TO</t>
+  </si>
+  <si>
+    <t>GGRO.TO</t>
+  </si>
+  <si>
+    <t>GEQT.TO</t>
+  </si>
+  <si>
+    <t>GBAL.TO</t>
+  </si>
+  <si>
+    <t>XGRO.TO</t>
+  </si>
+  <si>
+    <t>XBAL.TO</t>
+  </si>
+  <si>
+    <t>FIE.TO</t>
+  </si>
+  <si>
+    <t>XTR.TO</t>
+  </si>
+  <si>
+    <t>XCNS.TO</t>
+  </si>
+  <si>
+    <t>XEQT.TO</t>
+  </si>
+  <si>
+    <t>XINC.TO</t>
+  </si>
+  <si>
+    <t>CGR.TO</t>
+  </si>
+  <si>
+    <t>XRE.TO</t>
+  </si>
+  <si>
+    <t>Percentile:</t>
+  </si>
+  <si>
+    <t>&lt;15 % drop</t>
+  </si>
+  <si>
+    <t>&lt;20% drop</t>
+  </si>
+  <si>
+    <t>&lt;30</t>
+  </si>
+  <si>
+    <t>&lt;45</t>
+  </si>
+  <si>
+    <t>&lt;100</t>
+  </si>
+  <si>
+    <t>All Time Drawdown</t>
+  </si>
+  <si>
+    <t>10 year drawdown</t>
+  </si>
+  <si>
+    <t>average drawdown</t>
+  </si>
+  <si>
+    <t>start date</t>
+  </si>
+  <si>
+    <t>10 year % drop</t>
+  </si>
+  <si>
+    <t>All Time % drop</t>
   </si>
 </sst>
 </file>
@@ -1525,7 +2015,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1541,6 +2031,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1597,6 +2088,64 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>13</v>
+    <v>3</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4904,25 +5453,4357 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53375418-B1E3-EB4B-A330-963D77721972}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:N149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A1" t="str" cm="1">
+        <f t="array" ref="A1">_xlfn.TEXTJOIN(", ", TRUE, IF(all!E2:E170&lt;&gt;"", CHAR(34) &amp; all!E2:E170 &amp; ".TO" &amp; CHAR(34), ""))</f>
+        <v>"SVR.TO", "IBIT.TO", "CGL.TO", "XMV.TO", "XMI.TO", "XML.TO", "XIN.TO", "XMS.TO", "XMY.TO", "XEM.TO", "XMM.TO", "XEC.TO", "XUS.TO", "XEF.TO", "XMH.TO", "XMC.TO", "XDIV.TO", "XMU.TO", "XQQ.TO", "XWD.TO", "XDUH.TO", "XDG.TO", "XSU.TO", "XDU.TO", "XSUS.TO", "XSEA.TO", "XDGH.TO", "XESG.TO", "XGI.TO", "XCD.TO", "XSEM.TO", "XSP.TO", "CWO.TO", "CRQ.TO", "XID.TO", "XCH.TO", "XEMC.TO", "XHC.TO", "XDRV.TO", "CWW.TO", "XCV.TO", "XCG.TO", "XUSR.TO", "XDV.TO", "XDSR.TO", "XEU.TO", "CEW.TO", "XEH.TO", "XUU.TO", "COW.TO", "CIF.TO", "CYH.TO", "XDNA.TO", "XCLN.TO", "XQQU.TO", "XEXP.TO", "XAW.TO", "XHAK.TO", "XETM.TO", "XCHP.TO", "CIE.TO", "XUSF.TO", "XAD.TO", "XEN.TO", "CUD.TO", "CDZ.TO", "XQLT.TO", "XIU.TO", "CJP.TO", "XEG.TO", "XST.TO", "XIC.TO", "CPD.TO", "XSMC.TO", "XMA.TO", "XUSC.TO", "XSMH.TO", "XFH.TO", "XIT.TO", "XFN.TO", "XMTM.TO", "XBM.TO", "XEI.TO", "XVLU.TO", "XMD.TO", "XUT.TO", "XCSR.TO", "XPF.TO", "XHU.TO", "XGD.TO", "XSPC.TO", "XUH.TO", "XCS.TO", "XHD.TO", "CLU.TO", "XMW.TO", "XSC.TO", "XSE.TO", "CMR.TO", "CLG.TO", "CBH.TO", "CLF.TO", "CBO.TO", "XGGB.TO", "CVD.TO", "XQB.TO", "XAGG.TO", "XCBG.TO", "XSHG.TO", "XAGH.TO", "XSTB.TO", "XFLB.TO", "XFLI.TO", "XFLX.TO", "XSAB.TO", "XTLH.TO", "XTLT.TO", "XFR.TO", "XGB.TO", "XCB.TO", "XSB.TO", "XSI.TO", "XRB.TO", "XLB.TO", "XHB.TO", "XBB.TO", "XSH.TO", "XSTH.TO", "XSTP.TO", "XCBU.TO", "XIGS.TO", "XSHU.TO", "XEB.TO", "XIG.TO", "XHY.TO", "GCNS.TO", "GGRO.TO", "GEQT.TO", "GBAL.TO", "XGRO.TO", "XBAL.TO", "FIE.TO", "XTR.TO", "XCNS.TO", "XEQT.TO", "XINC.TO", "CGR.TO", "XRE.TO"</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B3" t="s">
+        <v>482</v>
+      </c>
+      <c r="C3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D3" t="s">
+        <v>480</v>
+      </c>
+      <c r="E3" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B4" s="7">
+        <v>40115</v>
+      </c>
+      <c r="C4">
+        <v>-77.851644714471902</v>
+      </c>
+      <c r="D4">
+        <v>-45.524957090810702</v>
+      </c>
+      <c r="E4">
+        <f>AVERAGE(C4,D4)</f>
+        <v>-61.688300902641302</v>
+      </c>
+      <c r="G4" t="s">
+        <v>473</v>
+      </c>
+      <c r="H4" t="s">
+        <v>484</v>
+      </c>
+      <c r="I4" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B5" s="7">
+        <v>40455</v>
+      </c>
+      <c r="C5">
+        <v>-45.9601897923569</v>
+      </c>
+      <c r="D5">
+        <v>-23.7209342814186</v>
+      </c>
+      <c r="E5">
+        <f>AVERAGE(C5,D5)</f>
+        <v>-34.840562036887746</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f>_xlfn.PERCENTILE.INC($C$4:$C$149,G5)</f>
+        <v>-90.613043189729098</v>
+      </c>
+      <c r="I5">
+        <f>_xlfn.PERCENTILE.INC($D$4:$D$149,G5)</f>
+        <v>-80.886426103414095</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B6" s="7">
+        <v>41124</v>
+      </c>
+      <c r="C6">
+        <v>-35.578329025495599</v>
+      </c>
+      <c r="D6">
+        <v>-35.578329025495599</v>
+      </c>
+      <c r="E6">
+        <f>AVERAGE(C6,D6)</f>
+        <v>-35.578329025495599</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:I9" si="0">_xlfn.PERCENTILE.INC($C$4:$C$149,G6)</f>
+        <v>-47.517735533489002</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I9" si="1">_xlfn.PERCENTILE.INC($D$4:$D$149,G6)</f>
+        <v>-39.930086105074899</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7" s="7">
+        <v>41138</v>
+      </c>
+      <c r="C7">
+        <v>-23.240714738193901</v>
+      </c>
+      <c r="D7">
+        <v>-23.240714738193901</v>
+      </c>
+      <c r="E7">
+        <f>AVERAGE(C7,D7)</f>
+        <v>-23.240714738193901</v>
+      </c>
+      <c r="G7">
+        <v>0.45</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>-34.343546597726345</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>-32.093989745851545</v>
+      </c>
+      <c r="J7" t="s">
+        <v>474</v>
+      </c>
+      <c r="K7" t="s">
+        <v>475</v>
+      </c>
+      <c r="L7" t="s">
+        <v>476</v>
+      </c>
+      <c r="M7" t="s">
+        <v>477</v>
+      </c>
+      <c r="N7" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>331</v>
+      </c>
+      <c r="B8" s="7">
+        <v>42471</v>
+      </c>
+      <c r="C8">
+        <v>-28.6226126347416</v>
+      </c>
+      <c r="D8">
+        <v>-28.6226126347416</v>
+      </c>
+      <c r="E8">
+        <f>AVERAGE(C8,D8)</f>
+        <v>-28.6226126347416</v>
+      </c>
+      <c r="G8">
+        <v>0.75</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>-22.615001173705473</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>-22.009800226432802</v>
+      </c>
+      <c r="J8" t="e" cm="1" vm="1">
+        <f t="array" ref="J8">_xlfn._xlws.FILTER($A$4:$A$149, ($C$4:$C$149 &gt;= -15) * ($C$4:$C$149 &lt;= I9))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K8" t="str" cm="1">
+        <f t="array" ref="K8:K33">_xlfn._xlws.FILTER($A$4:$A$149, ($C$4:$C$149 &gt;= -20) * ($C$4:$C$149 &lt;= 15))</f>
+        <v>XEMC.TO</v>
+      </c>
+      <c r="L8" t="str" cm="1">
+        <f t="array" ref="L8:L51">_xlfn._xlws.FILTER($A$4:$A$149, ($C$4:$C$149 &gt;= -30) * ($C$4:$C$149 &lt;= -20))</f>
+        <v>XMI.TO</v>
+      </c>
+      <c r="M8" t="str" cm="1">
+        <f t="array" ref="M8:M36">_xlfn._xlws.FILTER($A$4:$A$149, ($C$4:$C$149 &gt;= -45) * ($C$4:$C$149 &lt;= -35))</f>
+        <v>XMV.TO</v>
+      </c>
+      <c r="N8" t="str" cm="1">
+        <f t="array" ref="N8:N42">_xlfn._xlws.FILTER($A$4:$A$149, ($C$4:$C$149 &gt;= -100) * ($C$4:$C$149 &lt;= -45))</f>
+        <v>SVR.TO</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>332</v>
+      </c>
+      <c r="B9" s="7">
+        <v>37361</v>
+      </c>
+      <c r="C9">
+        <v>-60.540183851736003</v>
+      </c>
+      <c r="D9">
+        <v>-33.6749084240599</v>
+      </c>
+      <c r="E9">
+        <f>AVERAGE(C9,D9)</f>
+        <v>-47.107546137897955</v>
+      </c>
+      <c r="G9">
+        <v>0.9</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>-15.9482072722666</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>-15.182684784455649</v>
+      </c>
+      <c r="K9" t="str">
+        <v>XHAK.TO</v>
+      </c>
+      <c r="L9" t="str">
+        <v>XML.TO</v>
+      </c>
+      <c r="M9" t="str">
+        <v>XMS.TO</v>
+      </c>
+      <c r="N9" t="str">
+        <v>CGL.TO</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>333</v>
+      </c>
+      <c r="B10" s="7">
+        <v>42471</v>
+      </c>
+      <c r="C10">
+        <v>-36.482082960585302</v>
+      </c>
+      <c r="D10">
+        <v>-36.482082960585302</v>
+      </c>
+      <c r="E10">
+        <f>AVERAGE(C10,D10)</f>
+        <v>-36.482082960585302</v>
+      </c>
+      <c r="K10" t="str">
+        <v>XUSF.TO</v>
+      </c>
+      <c r="L10" t="str">
+        <v>XMY.TO</v>
+      </c>
+      <c r="M10" t="str">
+        <v>XEM.TO</v>
+      </c>
+      <c r="N10" t="str">
+        <v>XIN.TO</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>334</v>
+      </c>
+      <c r="B11" s="7">
+        <v>42535</v>
+      </c>
+      <c r="C11">
+        <v>-28.995599883853</v>
+      </c>
+      <c r="D11">
+        <v>-28.995599883853</v>
+      </c>
+      <c r="E11">
+        <f>AVERAGE(C11,D11)</f>
+        <v>-28.995599883853</v>
+      </c>
+      <c r="K11" t="str">
+        <v>XAD.TO</v>
+      </c>
+      <c r="L11" t="str">
+        <v>XMM.TO</v>
+      </c>
+      <c r="M11" t="str">
+        <v>XMH.TO</v>
+      </c>
+      <c r="N11" t="str">
+        <v>XSU.TO</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>335</v>
+      </c>
+      <c r="B12" s="7">
+        <v>40115</v>
+      </c>
+      <c r="C12">
+        <v>-36.912915260067003</v>
+      </c>
+      <c r="D12">
+        <v>-36.912915260067003</v>
+      </c>
+      <c r="E12">
+        <f>AVERAGE(C12,D12)</f>
+        <v>-36.912915260067003</v>
+      </c>
+      <c r="K12" t="str">
+        <v>XUSC.TO</v>
+      </c>
+      <c r="L12" t="str">
+        <v>XUS.TO</v>
+      </c>
+      <c r="M12" t="str">
+        <v>XMC.TO</v>
+      </c>
+      <c r="N12" t="str">
+        <v>XSP.TO</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>336</v>
+      </c>
+      <c r="B13" s="7">
+        <v>41137</v>
+      </c>
+      <c r="C13">
+        <v>-25.327947848096201</v>
+      </c>
+      <c r="D13">
+        <v>-25.327947848096201</v>
+      </c>
+      <c r="E13">
+        <f>AVERAGE(C13,D13)</f>
+        <v>-25.327947848096201</v>
+      </c>
+      <c r="K13" t="str">
+        <v>XSPC.TO</v>
+      </c>
+      <c r="L13" t="str">
+        <v>XEF.TO</v>
+      </c>
+      <c r="M13" t="str">
+        <v>XDIV.TO</v>
+      </c>
+      <c r="N13" t="str">
+        <v>XCH.TO</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>337</v>
+      </c>
+      <c r="B14" s="7">
+        <v>41379</v>
+      </c>
+      <c r="C14">
+        <v>-34.961740202497701</v>
+      </c>
+      <c r="D14">
+        <v>-34.961740202497701</v>
+      </c>
+      <c r="E14">
+        <f>AVERAGE(C14,D14)</f>
+        <v>-34.961740202497701</v>
+      </c>
+      <c r="K14" t="str">
+        <v>XSC.TO</v>
+      </c>
+      <c r="L14" t="str">
+        <v>XMU.TO</v>
+      </c>
+      <c r="M14" t="str">
+        <v>XQQ.TO</v>
+      </c>
+      <c r="N14" t="str">
+        <v>CWW.TO</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>338</v>
+      </c>
+      <c r="B15" s="7">
+        <v>41379</v>
+      </c>
+      <c r="C15">
+        <v>-27.226920635616601</v>
+      </c>
+      <c r="D15">
+        <v>-27.226920635616601</v>
+      </c>
+      <c r="E15">
+        <f>AVERAGE(C15,D15)</f>
+        <v>-27.226920635616601</v>
+      </c>
+      <c r="K15" t="str">
+        <v>CMR.TO</v>
+      </c>
+      <c r="L15" t="str">
+        <v>XWD.TO</v>
+      </c>
+      <c r="M15" t="str">
+        <v>XDUH.TO</v>
+      </c>
+      <c r="N15" t="str">
+        <v>XCV.TO</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>339</v>
+      </c>
+      <c r="B16" s="7">
+        <v>41379</v>
+      </c>
+      <c r="C16">
+        <v>-28.5051086362215</v>
+      </c>
+      <c r="D16">
+        <v>-28.5051086362215</v>
+      </c>
+      <c r="E16">
+        <f>AVERAGE(C16,D16)</f>
+        <v>-28.5051086362215</v>
+      </c>
+      <c r="K16" t="str">
+        <v>XAGG.TO</v>
+      </c>
+      <c r="L16" t="str">
+        <v>XDG.TO</v>
+      </c>
+      <c r="M16" t="str">
+        <v>XESG.TO</v>
+      </c>
+      <c r="N16" t="str">
+        <v>XCG.TO</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>340</v>
+      </c>
+      <c r="B17" s="7">
+        <v>42227</v>
+      </c>
+      <c r="C17">
+        <v>-44.824171426526298</v>
+      </c>
+      <c r="D17">
+        <v>-44.824171426526298</v>
+      </c>
+      <c r="E17">
+        <f>AVERAGE(C17,D17)</f>
+        <v>-44.824171426526298</v>
+      </c>
+      <c r="K17" t="str">
+        <v>XCBG.TO</v>
+      </c>
+      <c r="L17" t="str">
+        <v>XDU.TO</v>
+      </c>
+      <c r="M17" t="str">
+        <v>XGI.TO</v>
+      </c>
+      <c r="N17" t="str">
+        <v>XDV.TO</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>341</v>
+      </c>
+      <c r="B18" s="7">
+        <v>42226</v>
+      </c>
+      <c r="C18">
+        <v>-36.376405598032299</v>
+      </c>
+      <c r="D18">
+        <v>-36.376405598032299</v>
+      </c>
+      <c r="E18">
+        <f>AVERAGE(C18,D18)</f>
+        <v>-36.376405598032299</v>
+      </c>
+      <c r="K18" t="str">
+        <v>XSHG.TO</v>
+      </c>
+      <c r="L18" t="str">
+        <v>XSUS.TO</v>
+      </c>
+      <c r="M18" t="str">
+        <v>XCD.TO</v>
+      </c>
+      <c r="N18" t="str">
+        <v>CEW.TO</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>342</v>
+      </c>
+      <c r="B19" s="7">
+        <v>42901</v>
+      </c>
+      <c r="C19">
+        <v>-41.480206499419097</v>
+      </c>
+      <c r="D19">
+        <v>-41.480206499419097</v>
+      </c>
+      <c r="E19">
+        <f>AVERAGE(C19,D19)</f>
+        <v>-41.480206499419097</v>
+      </c>
+      <c r="K19" t="str">
+        <v>XSTB.TO</v>
+      </c>
+      <c r="L19" t="str">
+        <v>XSEA.TO</v>
+      </c>
+      <c r="M19" t="str">
+        <v>XSEM.TO</v>
+      </c>
+      <c r="N19" t="str">
+        <v>COW.TO</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>343</v>
+      </c>
+      <c r="B20" s="7">
+        <v>41124</v>
+      </c>
+      <c r="C20">
+        <v>-27.314885160028101</v>
+      </c>
+      <c r="D20">
+        <v>-27.314885160028101</v>
+      </c>
+      <c r="E20">
+        <f>AVERAGE(C20,D20)</f>
+        <v>-27.314885160028101</v>
+      </c>
+      <c r="K20" t="str">
+        <v>XFLI.TO</v>
+      </c>
+      <c r="L20" t="str">
+        <v>XHC.TO</v>
+      </c>
+      <c r="M20" t="str">
+        <v>CWO.TO</v>
+      </c>
+      <c r="N20" t="str">
+        <v>CYH.TO</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>344</v>
+      </c>
+      <c r="B21" s="7">
+        <v>40673</v>
+      </c>
+      <c r="C21">
+        <v>-38.694379572533201</v>
+      </c>
+      <c r="D21">
+        <v>-38.694379572533201</v>
+      </c>
+      <c r="E21">
+        <f>AVERAGE(C21,D21)</f>
+        <v>-38.694379572533201</v>
+      </c>
+      <c r="K21" t="str">
+        <v>XFLX.TO</v>
+      </c>
+      <c r="L21" t="str">
+        <v>XDRV.TO</v>
+      </c>
+      <c r="M21" t="str">
+        <v>CRQ.TO</v>
+      </c>
+      <c r="N21" t="str">
+        <v>XDNA.TO</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>345</v>
+      </c>
+      <c r="B22" s="7">
+        <v>40115</v>
+      </c>
+      <c r="C22">
+        <v>-27.481173775582</v>
+      </c>
+      <c r="D22">
+        <v>-27.481173775582</v>
+      </c>
+      <c r="E22">
+        <f>AVERAGE(C22,D22)</f>
+        <v>-27.481173775582</v>
+      </c>
+      <c r="K22" t="str">
+        <v>XTLH.TO</v>
+      </c>
+      <c r="L22" t="str">
+        <v>XUSR.TO</v>
+      </c>
+      <c r="M22" t="str">
+        <v>XID.TO</v>
+      </c>
+      <c r="N22" t="str">
+        <v>XCLN.TO</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>346</v>
+      </c>
+      <c r="B23" s="7">
+        <v>43109</v>
+      </c>
+      <c r="C23">
+        <v>-35.073070165420802</v>
+      </c>
+      <c r="D23">
+        <v>-35.073070165420802</v>
+      </c>
+      <c r="E23">
+        <f>AVERAGE(C23,D23)</f>
+        <v>-35.073070165420802</v>
+      </c>
+      <c r="K23" t="str">
+        <v>XFR.TO</v>
+      </c>
+      <c r="L23" t="str">
+        <v>XUU.TO</v>
+      </c>
+      <c r="M23" t="str">
+        <v>XEH.TO</v>
+      </c>
+      <c r="N23" t="str">
+        <v>XEN.TO</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>347</v>
+      </c>
+      <c r="B24" s="7">
+        <v>43109</v>
+      </c>
+      <c r="C24">
+        <v>-27.3420057939095</v>
+      </c>
+      <c r="D24">
+        <v>-27.3420057939095</v>
+      </c>
+      <c r="E24">
+        <f>AVERAGE(C24,D24)</f>
+        <v>-27.3420057939095</v>
+      </c>
+      <c r="K24" t="str">
+        <v>XSB.TO</v>
+      </c>
+      <c r="L24" t="str">
+        <v>XQQU.TO</v>
+      </c>
+      <c r="M24" t="str">
+        <v>CIF.TO</v>
+      </c>
+      <c r="N24" t="str">
+        <v>CDZ.TO</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>348</v>
+      </c>
+      <c r="B25" s="7">
+        <v>39220</v>
+      </c>
+      <c r="C25">
+        <v>-63.470756220725796</v>
+      </c>
+      <c r="D25">
+        <v>-45.4866778104182</v>
+      </c>
+      <c r="E25">
+        <f>AVERAGE(C25,D25)</f>
+        <v>-54.478717015572002</v>
+      </c>
+      <c r="K25" t="str">
+        <v>XSH.TO</v>
+      </c>
+      <c r="L25" t="str">
+        <v>XEXP.TO</v>
+      </c>
+      <c r="M25" t="str">
+        <v>XCHP.TO</v>
+      </c>
+      <c r="N25" t="str">
+        <v>XIU.TO</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>349</v>
+      </c>
+      <c r="B26" s="7">
+        <v>42901</v>
+      </c>
+      <c r="C26">
+        <v>-26.255147113317999</v>
+      </c>
+      <c r="D26">
+        <v>-26.255147113317999</v>
+      </c>
+      <c r="E26">
+        <f>AVERAGE(C26,D26)</f>
+        <v>-26.255147113317999</v>
+      </c>
+      <c r="K26" t="str">
+        <v>XSTH.TO</v>
+      </c>
+      <c r="L26" t="str">
+        <v>XAW.TO</v>
+      </c>
+      <c r="M26" t="str">
+        <v>CIE.TO</v>
+      </c>
+      <c r="N26" t="str">
+        <v>XEG.TO</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>350</v>
+      </c>
+      <c r="B27" s="7">
+        <v>43546</v>
+      </c>
+      <c r="C27">
+        <v>-28.322980097297499</v>
+      </c>
+      <c r="D27">
+        <v>-28.322980097297499</v>
+      </c>
+      <c r="E27">
+        <f>AVERAGE(C27,D27)</f>
+        <v>-28.322980097297499</v>
+      </c>
+      <c r="K27" t="str">
+        <v>XSTP.TO</v>
+      </c>
+      <c r="L27" t="str">
+        <v>XQLT.TO</v>
+      </c>
+      <c r="M27" t="str">
+        <v>CUD.TO</v>
+      </c>
+      <c r="N27" t="str">
+        <v>XIC.TO</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>351</v>
+      </c>
+      <c r="B28" s="7">
+        <v>43550</v>
+      </c>
+      <c r="C28">
+        <v>-29.765112616931599</v>
+      </c>
+      <c r="D28">
+        <v>-29.765112616931599</v>
+      </c>
+      <c r="E28">
+        <f>AVERAGE(C28,D28)</f>
+        <v>-29.765112616931599</v>
+      </c>
+      <c r="K28" t="str">
+        <v>XCBU.TO</v>
+      </c>
+      <c r="L28" t="str">
+        <v>XST.TO</v>
+      </c>
+      <c r="M28" t="str">
+        <v>CJP.TO</v>
+      </c>
+      <c r="N28" t="str">
+        <v>CPD.TO</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>352</v>
+      </c>
+      <c r="B29" s="7">
+        <v>43011</v>
+      </c>
+      <c r="C29">
+        <v>-33.2471971786238</v>
+      </c>
+      <c r="D29">
+        <v>-33.2471971786238</v>
+      </c>
+      <c r="E29">
+        <f>AVERAGE(C29,D29)</f>
+        <v>-33.2471971786238</v>
+      </c>
+      <c r="K29" t="str">
+        <v>XIGS.TO</v>
+      </c>
+      <c r="L29" t="str">
+        <v>XMTM.TO</v>
+      </c>
+      <c r="M29" t="str">
+        <v>XSMC.TO</v>
+      </c>
+      <c r="N29" t="str">
+        <v>XMA.TO</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>353</v>
+      </c>
+      <c r="B30" s="7">
+        <v>43559</v>
+      </c>
+      <c r="C30">
+        <v>-37.357635079051299</v>
+      </c>
+      <c r="D30">
+        <v>-37.357635079051299</v>
+      </c>
+      <c r="E30">
+        <f>AVERAGE(C30,D30)</f>
+        <v>-37.357635079051299</v>
+      </c>
+      <c r="K30" t="str">
+        <v>XSHU.TO</v>
+      </c>
+      <c r="L30" t="str">
+        <v>XCSR.TO</v>
+      </c>
+      <c r="M30" t="str">
+        <v>XUT.TO</v>
+      </c>
+      <c r="N30" t="str">
+        <v>XSMH.TO</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>354</v>
+      </c>
+      <c r="B31" s="7">
+        <v>41372</v>
+      </c>
+      <c r="C31">
+        <v>-41.430534621046299</v>
+      </c>
+      <c r="D31">
+        <v>-41.430534621046299</v>
+      </c>
+      <c r="E31">
+        <f>AVERAGE(C31,D31)</f>
+        <v>-41.430534621046299</v>
+      </c>
+      <c r="K31" t="str">
+        <v>GCNS.TO</v>
+      </c>
+      <c r="L31" t="str">
+        <v>XMW.TO</v>
+      </c>
+      <c r="M31" t="str">
+        <v>XUH.TO</v>
+      </c>
+      <c r="N31" t="str">
+        <v>XIT.TO</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>355</v>
+      </c>
+      <c r="B32" s="7">
+        <v>41372</v>
+      </c>
+      <c r="C32">
+        <v>-39.521105463480502</v>
+      </c>
+      <c r="D32">
+        <v>-39.521105463480502</v>
+      </c>
+      <c r="E32">
+        <f>AVERAGE(C32,D32)</f>
+        <v>-39.521105463480502</v>
+      </c>
+      <c r="K32" t="str">
+        <v>XCNS.TO</v>
+      </c>
+      <c r="L32" t="str">
+        <v>XSE.TO</v>
+      </c>
+      <c r="M32" t="str">
+        <v>XHD.TO</v>
+      </c>
+      <c r="N32" t="str">
+        <v>XFN.TO</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>356</v>
+      </c>
+      <c r="B33" s="7">
+        <v>43546</v>
+      </c>
+      <c r="C33">
+        <v>-38.9784954506367</v>
+      </c>
+      <c r="D33">
+        <v>-38.9784954506367</v>
+      </c>
+      <c r="E33">
+        <f>AVERAGE(C33,D33)</f>
+        <v>-38.9784954506367</v>
+      </c>
+      <c r="K33" t="str">
+        <v>XINC.TO</v>
+      </c>
+      <c r="L33" t="str">
+        <v>CLG.TO</v>
+      </c>
+      <c r="M33" t="str">
+        <v>CLU.TO</v>
+      </c>
+      <c r="N33" t="str">
+        <v>XBM.TO</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>357</v>
+      </c>
+      <c r="B34" s="7">
+        <v>37361</v>
+      </c>
+      <c r="C34">
+        <v>-59.009698325934103</v>
+      </c>
+      <c r="D34">
+        <v>-36.052424683510701</v>
+      </c>
+      <c r="E34">
+        <f>AVERAGE(C34,D34)</f>
+        <v>-47.531061504722402</v>
+      </c>
+      <c r="L34" t="str">
+        <v>CBH.TO</v>
+      </c>
+      <c r="M34" t="str">
+        <v>XLB.TO</v>
+      </c>
+      <c r="N34" t="str">
+        <v>XEI.TO</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>358</v>
+      </c>
+      <c r="B35" s="7">
+        <v>39910</v>
+      </c>
+      <c r="C35">
+        <v>-37.280346822895602</v>
+      </c>
+      <c r="D35">
+        <v>-34.848120360137003</v>
+      </c>
+      <c r="E35">
+        <f>AVERAGE(C35,D35)</f>
+        <v>-36.064233591516299</v>
+      </c>
+      <c r="L35" t="str">
+        <v>CLF.TO</v>
+      </c>
+      <c r="M35" t="str">
+        <v>XEB.TO</v>
+      </c>
+      <c r="N35" t="str">
+        <v>XMD.TO</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>359</v>
+      </c>
+      <c r="B36" s="7">
+        <v>39815</v>
+      </c>
+      <c r="C36">
+        <v>-41.750440743042503</v>
+      </c>
+      <c r="D36">
+        <v>-41.750440743042503</v>
+      </c>
+      <c r="E36">
+        <f>AVERAGE(C36,D36)</f>
+        <v>-41.750440743042503</v>
+      </c>
+      <c r="L36" t="str">
+        <v>CBO.TO</v>
+      </c>
+      <c r="M36" t="str">
+        <v>XHY.TO</v>
+      </c>
+      <c r="N36" t="str">
+        <v>XPF.TO</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>360</v>
+      </c>
+      <c r="B37" s="7">
+        <v>40205</v>
+      </c>
+      <c r="C37">
+        <v>-42.716533821834801</v>
+      </c>
+      <c r="D37">
+        <v>-39.714566023737397</v>
+      </c>
+      <c r="E37">
+        <f>AVERAGE(C37,D37)</f>
+        <v>-41.215549922786096</v>
+      </c>
+      <c r="L37" t="str">
+        <v>XQB.TO</v>
+      </c>
+      <c r="N37" t="str">
+        <v>XGD.TO</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>361</v>
+      </c>
+      <c r="B38" s="7">
+        <v>40205</v>
+      </c>
+      <c r="C38">
+        <v>-58.9673895203398</v>
+      </c>
+      <c r="D38">
+        <v>-58.9673895203398</v>
+      </c>
+      <c r="E38">
+        <f>AVERAGE(C38,D38)</f>
+        <v>-58.9673895203398</v>
+      </c>
+      <c r="L38" t="str">
+        <v>XAGH.TO</v>
+      </c>
+      <c r="N38" t="str">
+        <v>XCS.TO</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>362</v>
+      </c>
+      <c r="B39" s="7">
+        <v>44972</v>
+      </c>
+      <c r="C39">
+        <v>-15.9023198161371</v>
+      </c>
+      <c r="D39">
+        <v>-15.9023198161371</v>
+      </c>
+      <c r="E39">
+        <f>AVERAGE(C39,D39)</f>
+        <v>-15.9023198161371</v>
+      </c>
+      <c r="L39" t="str">
+        <v>XFLB.TO</v>
+      </c>
+      <c r="N39" t="str">
+        <v>XGRO.TO</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>363</v>
+      </c>
+      <c r="B40" s="7">
+        <v>40932</v>
+      </c>
+      <c r="C40">
+        <v>-27.282451007960699</v>
+      </c>
+      <c r="D40">
+        <v>-27.282451007960699</v>
+      </c>
+      <c r="E40">
+        <f>AVERAGE(C40,D40)</f>
+        <v>-27.282451007960699</v>
+      </c>
+      <c r="L40" t="str">
+        <v>XSAB.TO</v>
+      </c>
+      <c r="N40" t="str">
+        <v>FIE.TO</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>364</v>
+      </c>
+      <c r="B41" s="7">
+        <v>44978</v>
+      </c>
+      <c r="C41">
+        <v>-28.0163564794425</v>
+      </c>
+      <c r="D41">
+        <v>-28.0163564794425</v>
+      </c>
+      <c r="E41">
+        <f>AVERAGE(C41,D41)</f>
+        <v>-28.0163564794425</v>
+      </c>
+      <c r="L41" t="str">
+        <v>XTLT.TO</v>
+      </c>
+      <c r="N41" t="str">
+        <v>XTR.TO</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>365</v>
+      </c>
+      <c r="B42" s="7">
+        <v>39380</v>
+      </c>
+      <c r="C42">
+        <v>-47.517735533489002</v>
+      </c>
+      <c r="D42">
+        <v>-31.9446882809033</v>
+      </c>
+      <c r="E42">
+        <f>AVERAGE(C42,D42)</f>
+        <v>-39.731211907196155</v>
+      </c>
+      <c r="L42" t="str">
+        <v>XGB.TO</v>
+      </c>
+      <c r="N42" t="str">
+        <v>XRE.TO</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>366</v>
+      </c>
+      <c r="B43" s="7">
+        <v>39031</v>
+      </c>
+      <c r="C43">
+        <v>-54.518073154371301</v>
+      </c>
+      <c r="D43">
+        <v>-42.061178522003402</v>
+      </c>
+      <c r="E43">
+        <f>AVERAGE(C43,D43)</f>
+        <v>-48.289625838187348</v>
+      </c>
+      <c r="L43" t="str">
+        <v>XCB.TO</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>367</v>
+      </c>
+      <c r="B44" s="7">
+        <v>39031</v>
+      </c>
+      <c r="C44">
+        <v>-52.733330232450598</v>
+      </c>
+      <c r="D44">
+        <v>-32.143756900834298</v>
+      </c>
+      <c r="E44">
+        <f>AVERAGE(C44,D44)</f>
+        <v>-42.438543566642451</v>
+      </c>
+      <c r="L44" t="str">
+        <v>XSI.TO</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>368</v>
+      </c>
+      <c r="B45" s="7">
+        <v>43944</v>
+      </c>
+      <c r="C45">
+        <v>-28.705181478818599</v>
+      </c>
+      <c r="D45">
+        <v>-28.705181478818599</v>
+      </c>
+      <c r="E45">
+        <f>AVERAGE(C45,D45)</f>
+        <v>-28.705181478818599</v>
+      </c>
+      <c r="L45" t="str">
+        <v>XRB.TO</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>369</v>
+      </c>
+      <c r="B46" s="7">
+        <v>38714</v>
+      </c>
+      <c r="C46">
+        <v>-52.969893255864299</v>
+      </c>
+      <c r="D46">
+        <v>-39.297725217707601</v>
+      </c>
+      <c r="E46">
+        <f>AVERAGE(C46,D46)</f>
+        <v>-46.13380923678595</v>
+      </c>
+      <c r="L46" t="str">
+        <v>XHB.TO</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>370</v>
+      </c>
+      <c r="B47" s="7">
+        <v>43956</v>
+      </c>
+      <c r="C47">
+        <v>-30.885389351795801</v>
+      </c>
+      <c r="D47">
+        <v>-30.885389351795801</v>
+      </c>
+      <c r="E47">
+        <f>AVERAGE(C47,D47)</f>
+        <v>-30.885389351795801</v>
+      </c>
+      <c r="L47" t="str">
+        <v>XBB.TO</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>371</v>
+      </c>
+      <c r="B48" s="7">
+        <v>41752</v>
+      </c>
+      <c r="C48">
+        <v>-32.602740400959703</v>
+      </c>
+      <c r="D48">
+        <v>-32.602740400959703</v>
+      </c>
+      <c r="E48">
+        <f>AVERAGE(C48,D48)</f>
+        <v>-32.602740400959703</v>
+      </c>
+      <c r="L48" t="str">
+        <v>GGRO.TO</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>372</v>
+      </c>
+      <c r="B49" s="7">
+        <v>39491</v>
+      </c>
+      <c r="C49">
+        <v>-54.945048714386303</v>
+      </c>
+      <c r="D49">
+        <v>-43.803418550265597</v>
+      </c>
+      <c r="E49">
+        <f>AVERAGE(C49,D49)</f>
+        <v>-49.374233632325954</v>
+      </c>
+      <c r="L49" t="str">
+        <v>GEQT.TO</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>373</v>
+      </c>
+      <c r="B50" s="7">
+        <v>41753</v>
+      </c>
+      <c r="C50">
+        <v>-35.813273249084801</v>
+      </c>
+      <c r="D50">
+        <v>-35.813273249084801</v>
+      </c>
+      <c r="E50">
+        <f>AVERAGE(C50,D50)</f>
+        <v>-35.813273249084801</v>
+      </c>
+      <c r="L50" t="str">
+        <v>GBAL.TO</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>374</v>
+      </c>
+      <c r="B51" s="7">
+        <v>42055</v>
+      </c>
+      <c r="C51">
+        <v>-28.217231768210699</v>
+      </c>
+      <c r="D51">
+        <v>-28.217231768210699</v>
+      </c>
+      <c r="E51">
+        <f>AVERAGE(C51,D51)</f>
+        <v>-28.217231768210699</v>
+      </c>
+      <c r="L51" t="str">
+        <v>XEQT.TO</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>375</v>
+      </c>
+      <c r="B52" s="7">
+        <v>39435</v>
+      </c>
+      <c r="C52">
+        <v>-55.001779542327199</v>
+      </c>
+      <c r="D52">
+        <v>-37.259340871880497</v>
+      </c>
+      <c r="E52">
+        <f>AVERAGE(C52,D52)</f>
+        <v>-46.130560207103848</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>376</v>
+      </c>
+      <c r="B53" s="7">
+        <v>39841</v>
+      </c>
+      <c r="C53">
+        <v>-42.3723244617793</v>
+      </c>
+      <c r="D53">
+        <v>-42.3723244617793</v>
+      </c>
+      <c r="E53">
+        <f>AVERAGE(C53,D53)</f>
+        <v>-42.3723244617793</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>377</v>
+      </c>
+      <c r="B54" s="7">
+        <v>39464</v>
+      </c>
+      <c r="C54">
+        <v>-63.497758961051801</v>
+      </c>
+      <c r="D54">
+        <v>-42.881041493921003</v>
+      </c>
+      <c r="E54">
+        <f>AVERAGE(C54,D54)</f>
+        <v>-53.189400227486402</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
+        <v>378</v>
+      </c>
+      <c r="B55" s="7">
+        <v>44685</v>
+      </c>
+      <c r="C55">
+        <v>-46.108441814651499</v>
+      </c>
+      <c r="D55">
+        <v>-46.108441814651499</v>
+      </c>
+      <c r="E55">
+        <f>AVERAGE(C55,D55)</f>
+        <v>-46.108441814651499</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>379</v>
+      </c>
+      <c r="B56" s="7">
+        <v>44685</v>
+      </c>
+      <c r="C56">
+        <v>-50.367281059887503</v>
+      </c>
+      <c r="D56">
+        <v>-50.367281059887503</v>
+      </c>
+      <c r="E56">
+        <f>AVERAGE(C56,D56)</f>
+        <v>-50.367281059887503</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>380</v>
+      </c>
+      <c r="B57" s="7">
+        <v>45182</v>
+      </c>
+      <c r="C57">
+        <v>-22.683706459665501</v>
+      </c>
+      <c r="D57">
+        <v>-22.683706459665501</v>
+      </c>
+      <c r="E57">
+        <f>AVERAGE(C57,D57)</f>
+        <v>-22.683706459665501</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>381</v>
+      </c>
+      <c r="B58" s="7">
+        <v>44712</v>
+      </c>
+      <c r="C58">
+        <v>-22.4384825770038</v>
+      </c>
+      <c r="D58">
+        <v>-22.4384825770038</v>
+      </c>
+      <c r="E58">
+        <f>AVERAGE(C58,D58)</f>
+        <v>-22.4384825770038</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>382</v>
+      </c>
+      <c r="B59" s="7">
+        <v>42055</v>
+      </c>
+      <c r="C59">
+        <v>-27.322589278399001</v>
+      </c>
+      <c r="D59">
+        <v>-27.322589278399001</v>
+      </c>
+      <c r="E59">
+        <f>AVERAGE(C59,D59)</f>
+        <v>-27.322589278399001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>383</v>
+      </c>
+      <c r="B60" s="7">
+        <v>44685</v>
+      </c>
+      <c r="C60">
+        <v>-17.956657508197502</v>
+      </c>
+      <c r="D60">
+        <v>-17.956657508197502</v>
+      </c>
+      <c r="E60">
+        <f>AVERAGE(C60,D60)</f>
+        <v>-17.956657508197502</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>384</v>
+      </c>
+      <c r="B61" s="7">
+        <v>45182</v>
+      </c>
+      <c r="C61">
+        <v>-34.1637792675334</v>
+      </c>
+      <c r="D61">
+        <v>-34.1637792675334</v>
+      </c>
+      <c r="E61">
+        <f>AVERAGE(C61,D61)</f>
+        <v>-34.1637792675334</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>385</v>
+      </c>
+      <c r="B62" s="7">
+        <v>45183</v>
+      </c>
+      <c r="C62">
+        <v>-39.063994006273703</v>
+      </c>
+      <c r="D62">
+        <v>-39.063994006273703</v>
+      </c>
+      <c r="E62">
+        <f>AVERAGE(C62,D62)</f>
+        <v>-39.063994006273703</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>386</v>
+      </c>
+      <c r="B63" s="7">
+        <v>39815</v>
+      </c>
+      <c r="C63">
+        <v>-43.859649431784398</v>
+      </c>
+      <c r="D63">
+        <v>-43.859649431784398</v>
+      </c>
+      <c r="E63">
+        <f>AVERAGE(C63,D63)</f>
+        <v>-43.859649431784398</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
+        <v>387</v>
+      </c>
+      <c r="B64" s="7">
+        <v>45175</v>
+      </c>
+      <c r="C64">
+        <v>-17.056564702487101</v>
+      </c>
+      <c r="D64">
+        <v>-17.056564702487101</v>
+      </c>
+      <c r="E64">
+        <f>AVERAGE(C64,D64)</f>
+        <v>-17.056564702487101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>388</v>
+      </c>
+      <c r="B65" s="7">
+        <v>45188</v>
+      </c>
+      <c r="C65">
+        <v>-16.059376459147401</v>
+      </c>
+      <c r="D65">
+        <v>-16.059376459147401</v>
+      </c>
+      <c r="E65">
+        <f>AVERAGE(C65,D65)</f>
+        <v>-16.059376459147401</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>389</v>
+      </c>
+      <c r="B66" s="7">
+        <v>39220</v>
+      </c>
+      <c r="C66">
+        <v>-50.898202224999999</v>
+      </c>
+      <c r="D66">
+        <v>-36.243881337501499</v>
+      </c>
+      <c r="E66">
+        <f>AVERAGE(C66,D66)</f>
+        <v>-43.571041781250749</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>390</v>
+      </c>
+      <c r="B67" s="7">
+        <v>40813</v>
+      </c>
+      <c r="C67">
+        <v>-38.454880219767396</v>
+      </c>
+      <c r="D67">
+        <v>-38.454880219767396</v>
+      </c>
+      <c r="E67">
+        <f>AVERAGE(C67,D67)</f>
+        <v>-38.454880219767396</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>391</v>
+      </c>
+      <c r="B68" s="7">
+        <v>38968</v>
+      </c>
+      <c r="C68">
+        <v>-52.7303711914046</v>
+      </c>
+      <c r="D68">
+        <v>-45.858186064969097</v>
+      </c>
+      <c r="E68">
+        <f>AVERAGE(C68,D68)</f>
+        <v>-49.294278628186845</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A69" t="s">
+        <v>392</v>
+      </c>
+      <c r="B69" s="7">
+        <v>43720</v>
+      </c>
+      <c r="C69">
+        <v>-25.292589820400998</v>
+      </c>
+      <c r="D69">
+        <v>-25.292589820400998</v>
+      </c>
+      <c r="E69">
+        <f>AVERAGE(C69,D69)</f>
+        <v>-25.292589820400998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>393</v>
+      </c>
+      <c r="B70" s="7">
+        <v>36437</v>
+      </c>
+      <c r="C70">
+        <v>-53.984208851521402</v>
+      </c>
+      <c r="D70">
+        <v>-35.925928751627602</v>
+      </c>
+      <c r="E70">
+        <f>AVERAGE(C70,D70)</f>
+        <v>-44.955068801574498</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>394</v>
+      </c>
+      <c r="B71" s="7">
+        <v>39815</v>
+      </c>
+      <c r="C71">
+        <v>-40.6555488382173</v>
+      </c>
+      <c r="D71">
+        <v>-40.6555488382173</v>
+      </c>
+      <c r="E71">
+        <f>AVERAGE(C71,D71)</f>
+        <v>-40.6555488382173</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>395</v>
+      </c>
+      <c r="B72" s="7">
+        <v>36973</v>
+      </c>
+      <c r="C72">
+        <v>-90.613043189729098</v>
+      </c>
+      <c r="D72">
+        <v>-80.886426103414095</v>
+      </c>
+      <c r="E72">
+        <f>AVERAGE(C72,D72)</f>
+        <v>-85.749734646571596</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>396</v>
+      </c>
+      <c r="B73" s="7">
+        <v>40932</v>
+      </c>
+      <c r="C73">
+        <v>-22.866493647348801</v>
+      </c>
+      <c r="D73">
+        <v>-22.866493647348801</v>
+      </c>
+      <c r="E73">
+        <f>AVERAGE(C73,D73)</f>
+        <v>-22.866493647348801</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>397</v>
+      </c>
+      <c r="B74" s="7">
+        <v>36944</v>
+      </c>
+      <c r="C74">
+        <v>-49.527213750271898</v>
+      </c>
+      <c r="D74">
+        <v>-37.211734870738503</v>
+      </c>
+      <c r="E74">
+        <f>AVERAGE(C74,D74)</f>
+        <v>-43.369474310505197</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>398</v>
+      </c>
+      <c r="B75" s="7">
+        <v>39380</v>
+      </c>
+      <c r="C75">
+        <v>-58.465608131885098</v>
+      </c>
+      <c r="D75">
+        <v>-46.232878770361097</v>
+      </c>
+      <c r="E75">
+        <f>AVERAGE(C75,D75)</f>
+        <v>-52.349243451123101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
+        <v>399</v>
+      </c>
+      <c r="B76" s="7">
+        <v>43720</v>
+      </c>
+      <c r="C76">
+        <v>-37.2987474281502</v>
+      </c>
+      <c r="D76">
+        <v>-37.2987474281502</v>
+      </c>
+      <c r="E76">
+        <f>AVERAGE(C76,D76)</f>
+        <v>-37.2987474281502</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A77" t="s">
+        <v>400</v>
+      </c>
+      <c r="B77" s="7">
+        <v>38714</v>
+      </c>
+      <c r="C77">
+        <v>-66.199440078200496</v>
+      </c>
+      <c r="D77">
+        <v>-33.419580746849903</v>
+      </c>
+      <c r="E77">
+        <f>AVERAGE(C77,D77)</f>
+        <v>-49.809510412525199</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A78" t="s">
+        <v>401</v>
+      </c>
+      <c r="B78" s="7">
+        <v>45491</v>
+      </c>
+      <c r="C78">
+        <v>-18.308668048828999</v>
+      </c>
+      <c r="D78">
+        <v>-18.308668048828999</v>
+      </c>
+      <c r="E78">
+        <f>AVERAGE(C78,D78)</f>
+        <v>-18.308668048828999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A79" t="s">
+        <v>402</v>
+      </c>
+      <c r="B79" s="7">
+        <v>43720</v>
+      </c>
+      <c r="C79">
+        <v>-45.434300295337401</v>
+      </c>
+      <c r="D79">
+        <v>-45.434300295337401</v>
+      </c>
+      <c r="E79">
+        <f>AVERAGE(C79,D79)</f>
+        <v>-45.434300295337401</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A80" t="s">
+        <v>403</v>
+      </c>
+      <c r="B80" s="7">
+        <v>42055</v>
+      </c>
+      <c r="C80">
+        <v>-33.854165773116598</v>
+      </c>
+      <c r="D80">
+        <v>-33.854165773116598</v>
+      </c>
+      <c r="E80">
+        <f>AVERAGE(C80,D80)</f>
+        <v>-33.854165773116598</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A81" t="s">
+        <v>404</v>
+      </c>
+      <c r="B81" s="7">
+        <v>36973</v>
+      </c>
+      <c r="C81">
+        <v>-81.203003933910296</v>
+      </c>
+      <c r="D81">
+        <v>-54.152829932372804</v>
+      </c>
+      <c r="E81">
+        <f>AVERAGE(C81,D81)</f>
+        <v>-67.677916933141546</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A82" t="s">
+        <v>405</v>
+      </c>
+      <c r="B82" s="7">
+        <v>36979</v>
+      </c>
+      <c r="C82">
+        <v>-58.907489524538803</v>
+      </c>
+      <c r="D82">
+        <v>-40.057433146039799</v>
+      </c>
+      <c r="E82">
+        <f>AVERAGE(C82,D82)</f>
+        <v>-49.482461335289301</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A83" t="s">
+        <v>406</v>
+      </c>
+      <c r="B83" s="7">
+        <v>43725</v>
+      </c>
+      <c r="C83">
+        <v>-29.234420509114699</v>
+      </c>
+      <c r="D83">
+        <v>-29.234420509114699</v>
+      </c>
+      <c r="E83">
+        <f>AVERAGE(C83,D83)</f>
+        <v>-29.234420509114699</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A84" t="s">
+        <v>407</v>
+      </c>
+      <c r="B84" s="7">
+        <v>40932</v>
+      </c>
+      <c r="C84">
+        <v>-63.916254657965901</v>
+      </c>
+      <c r="D84">
+        <v>-59.961311886503204</v>
+      </c>
+      <c r="E84">
+        <f>AVERAGE(C84,D84)</f>
+        <v>-61.938783272234552</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A85" t="s">
+        <v>408</v>
+      </c>
+      <c r="B85" s="7">
+        <v>40932</v>
+      </c>
+      <c r="C85">
+        <v>-47.359666324216199</v>
+      </c>
+      <c r="D85">
+        <v>-45.711835278359999</v>
+      </c>
+      <c r="E85">
+        <f>AVERAGE(C85,D85)</f>
+        <v>-46.535750801288103</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A86" t="s">
+        <v>409</v>
+      </c>
+      <c r="B86" s="7">
+        <v>43720</v>
+      </c>
+      <c r="C86">
+        <v>-34.403469041123998</v>
+      </c>
+      <c r="D86">
+        <v>-34.403469041123998</v>
+      </c>
+      <c r="E86">
+        <f>AVERAGE(C86,D86)</f>
+        <v>-34.403469041123998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A87" t="s">
+        <v>410</v>
+      </c>
+      <c r="B87" s="7">
+        <v>36958</v>
+      </c>
+      <c r="C87">
+        <v>-56.254467457278501</v>
+      </c>
+      <c r="D87">
+        <v>-43.4042567150506</v>
+      </c>
+      <c r="E87">
+        <f>AVERAGE(C87,D87)</f>
+        <v>-49.829362086164551</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A88" t="s">
+        <v>411</v>
+      </c>
+      <c r="B88" s="7">
+        <v>40932</v>
+      </c>
+      <c r="C88">
+        <v>-37.810943510133299</v>
+      </c>
+      <c r="D88">
+        <v>-37.810943510133299</v>
+      </c>
+      <c r="E88">
+        <f>AVERAGE(C88,D88)</f>
+        <v>-37.810943510133299</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A89" t="s">
+        <v>412</v>
+      </c>
+      <c r="B89" s="7">
+        <v>43944</v>
+      </c>
+      <c r="C89">
+        <v>-25.335910650557</v>
+      </c>
+      <c r="D89">
+        <v>-25.335910650557</v>
+      </c>
+      <c r="E89">
+        <f>AVERAGE(C89,D89)</f>
+        <v>-25.335910650557</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A90" t="s">
+        <v>413</v>
+      </c>
+      <c r="B90" s="7">
+        <v>40504</v>
+      </c>
+      <c r="C90">
+        <v>-53.414043277140898</v>
+      </c>
+      <c r="D90">
+        <v>-48.556152443456298</v>
+      </c>
+      <c r="E90">
+        <f>AVERAGE(C90,D90)</f>
+        <v>-50.985097860298595</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A91" t="s">
+        <v>414</v>
+      </c>
+      <c r="B91" s="7">
+        <v>42055</v>
+      </c>
+      <c r="C91">
+        <v>-30.407176277073201</v>
+      </c>
+      <c r="D91">
+        <v>-30.407176277073201</v>
+      </c>
+      <c r="E91">
+        <f>AVERAGE(C91,D91)</f>
+        <v>-30.407176277073201</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A92" t="s">
+        <v>415</v>
+      </c>
+      <c r="B92" s="7">
+        <v>36979</v>
+      </c>
+      <c r="C92">
+        <v>-73.671066950929401</v>
+      </c>
+      <c r="D92">
+        <v>-47.135563593419</v>
+      </c>
+      <c r="E92">
+        <f>AVERAGE(C92,D92)</f>
+        <v>-60.403315272174197</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A93" t="s">
+        <v>416</v>
+      </c>
+      <c r="B93" s="7">
+        <v>45492</v>
+      </c>
+      <c r="C93">
+        <v>-17.676089601741499</v>
+      </c>
+      <c r="D93">
+        <v>-17.676089601741499</v>
+      </c>
+      <c r="E93">
+        <f>AVERAGE(C93,D93)</f>
+        <v>-17.676089601741499</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A94" t="s">
+        <v>417</v>
+      </c>
+      <c r="B94" s="7">
+        <v>42055</v>
+      </c>
+      <c r="C94">
+        <v>-38.3656034020349</v>
+      </c>
+      <c r="D94">
+        <v>-38.3656034020349</v>
+      </c>
+      <c r="E94">
+        <f>AVERAGE(C94,D94)</f>
+        <v>-38.3656034020349</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A95" t="s">
+        <v>418</v>
+      </c>
+      <c r="B95" s="7">
+        <v>39220</v>
+      </c>
+      <c r="C95">
+        <v>-62.865358256558601</v>
+      </c>
+      <c r="D95">
+        <v>-53.318335973745199</v>
+      </c>
+      <c r="E95">
+        <f>AVERAGE(C95,D95)</f>
+        <v>-58.0918471151519</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A96" t="s">
+        <v>419</v>
+      </c>
+      <c r="B96" s="7">
+        <v>41141</v>
+      </c>
+      <c r="C96">
+        <v>-39.179224984677298</v>
+      </c>
+      <c r="D96">
+        <v>-39.179224984677298</v>
+      </c>
+      <c r="E96">
+        <f>AVERAGE(C96,D96)</f>
+        <v>-39.179224984677298</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A97" t="s">
+        <v>420</v>
+      </c>
+      <c r="B97" s="7">
+        <v>39815</v>
+      </c>
+      <c r="C97">
+        <v>-39.930086105074899</v>
+      </c>
+      <c r="D97">
+        <v>-39.930086105074899</v>
+      </c>
+      <c r="E97">
+        <f>AVERAGE(C97,D97)</f>
+        <v>-39.930086105074899</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A98" t="s">
+        <v>421</v>
+      </c>
+      <c r="B98" s="7">
+        <v>41134</v>
+      </c>
+      <c r="C98">
+        <v>-21.420925357565601</v>
+      </c>
+      <c r="D98">
+        <v>-21.420925357565601</v>
+      </c>
+      <c r="E98">
+        <f>AVERAGE(C98,D98)</f>
+        <v>-21.420925357565601</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A99" t="s">
+        <v>422</v>
+      </c>
+      <c r="B99" s="7">
+        <v>42269</v>
+      </c>
+      <c r="C99">
+        <v>-15.994094728396099</v>
+      </c>
+      <c r="D99">
+        <v>-15.994094728396099</v>
+      </c>
+      <c r="E99">
+        <f>AVERAGE(C99,D99)</f>
+        <v>-15.994094728396099</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A100" t="s">
+        <v>423</v>
+      </c>
+      <c r="B100" s="7">
+        <v>42640</v>
+      </c>
+      <c r="C100">
+        <v>-23.246216501478202</v>
+      </c>
+      <c r="D100">
+        <v>-23.246216501478202</v>
+      </c>
+      <c r="E100">
+        <f>AVERAGE(C100,D100)</f>
+        <v>-23.246216501478202</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A101" t="s">
+        <v>424</v>
+      </c>
+      <c r="B101" s="7">
+        <v>39497</v>
+      </c>
+      <c r="C101">
+        <v>-0.81705828002918501</v>
+      </c>
+      <c r="D101">
+        <v>-0.51730666577004303</v>
+      </c>
+      <c r="E101">
+        <f>AVERAGE(C101,D101)</f>
+        <v>-0.66718247289961408</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A102" t="s">
+        <v>425</v>
+      </c>
+      <c r="B102" s="7">
+        <v>40952</v>
+      </c>
+      <c r="C102">
+        <v>-20.930231241258301</v>
+      </c>
+      <c r="D102">
+        <v>-19.899754731228299</v>
+      </c>
+      <c r="E102">
+        <f>AVERAGE(C102,D102)</f>
+        <v>-20.414992986243298</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A103" t="s">
+        <v>426</v>
+      </c>
+      <c r="B103" s="7">
+        <v>40952</v>
+      </c>
+      <c r="C103">
+        <v>-20.910873858031</v>
+      </c>
+      <c r="D103">
+        <v>-19.731615582051699</v>
+      </c>
+      <c r="E103">
+        <f>AVERAGE(C103,D103)</f>
+        <v>-20.321244720041349</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A104" t="s">
+        <v>427</v>
+      </c>
+      <c r="B104" s="7">
+        <v>39491</v>
+      </c>
+      <c r="C104">
+        <v>-25.662096026383001</v>
+      </c>
+      <c r="D104">
+        <v>-16.125704200785499</v>
+      </c>
+      <c r="E104">
+        <f>AVERAGE(C104,D104)</f>
+        <v>-20.893900113584252</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A105" t="s">
+        <v>428</v>
+      </c>
+      <c r="B105" s="7">
+        <v>40151</v>
+      </c>
+      <c r="C105">
+        <v>-20.343022888638099</v>
+      </c>
+      <c r="D105">
+        <v>-14.475703499472599</v>
+      </c>
+      <c r="E105">
+        <f>AVERAGE(C105,D105)</f>
+        <v>-17.409363194055349</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A106" t="s">
+        <v>429</v>
+      </c>
+      <c r="B106" s="7">
+        <v>40708</v>
+      </c>
+      <c r="C106">
+        <v>-30.1127983003549</v>
+      </c>
+      <c r="D106">
+        <v>-26.089214250545002</v>
+      </c>
+      <c r="E106">
+        <f>AVERAGE(C106,D106)</f>
+        <v>-28.101006275449951</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A107" t="s">
+        <v>430</v>
+      </c>
+      <c r="B107" s="7">
+        <v>40288</v>
+      </c>
+      <c r="C107">
+        <v>-21.874998669539099</v>
+      </c>
+      <c r="D107">
+        <v>-21.874998669539099</v>
+      </c>
+      <c r="E107">
+        <f>AVERAGE(C107,D107)</f>
+        <v>-21.874998669539099</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A108" t="s">
+        <v>431</v>
+      </c>
+      <c r="B108" s="7">
+        <v>45309</v>
+      </c>
+      <c r="C108">
+        <v>-7.7443609885170899</v>
+      </c>
+      <c r="D108">
+        <v>-7.7443609885170899</v>
+      </c>
+      <c r="E108">
+        <f>AVERAGE(C108,D108)</f>
+        <v>-7.7443609885170899</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A109" t="s">
+        <v>432</v>
+      </c>
+      <c r="B109" s="7">
+        <v>44404</v>
+      </c>
+      <c r="C109">
+        <v>-14.7497589414471</v>
+      </c>
+      <c r="D109">
+        <v>-14.7497589414471</v>
+      </c>
+      <c r="E109">
+        <f>AVERAGE(C109,D109)</f>
+        <v>-14.7497589414471</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A110" t="s">
+        <v>433</v>
+      </c>
+      <c r="B110" s="7">
+        <v>44404</v>
+      </c>
+      <c r="C110">
+        <v>-9.9237979917659995</v>
+      </c>
+      <c r="D110">
+        <v>-9.9237979917659995</v>
+      </c>
+      <c r="E110">
+        <f>AVERAGE(C110,D110)</f>
+        <v>-9.9237979917659995</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A111" t="s">
+        <v>434</v>
+      </c>
+      <c r="B111" s="7">
+        <v>44404</v>
+      </c>
+      <c r="C111">
+        <v>-21.840797313466201</v>
+      </c>
+      <c r="D111">
+        <v>-21.840797313466201</v>
+      </c>
+      <c r="E111">
+        <f>AVERAGE(C111,D111)</f>
+        <v>-21.840797313466201</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A112" t="s">
+        <v>435</v>
+      </c>
+      <c r="B112" s="7">
+        <v>43565</v>
+      </c>
+      <c r="C112">
+        <v>-9.97566575751258</v>
+      </c>
+      <c r="D112">
+        <v>-9.97566575751258</v>
+      </c>
+      <c r="E112">
+        <f>AVERAGE(C112,D112)</f>
+        <v>-9.97566575751258</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A113" t="s">
+        <v>436</v>
+      </c>
+      <c r="B113" s="7">
+        <v>44964</v>
+      </c>
+      <c r="C113">
+        <v>-21.7819930246952</v>
+      </c>
+      <c r="D113">
+        <v>-21.7819930246952</v>
+      </c>
+      <c r="E113">
+        <f>AVERAGE(C113,D113)</f>
+        <v>-21.7819930246952</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A114" t="s">
+        <v>437</v>
+      </c>
+      <c r="B114" s="7">
+        <v>45561</v>
+      </c>
+      <c r="C114">
+        <v>-7.3532851978418998</v>
+      </c>
+      <c r="D114">
+        <v>-7.3532851978418998</v>
+      </c>
+      <c r="E114">
+        <f>AVERAGE(C114,D114)</f>
+        <v>-7.3532851978418998</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A115" t="s">
+        <v>438</v>
+      </c>
+      <c r="B115" s="7">
+        <v>45569</v>
+      </c>
+      <c r="C115">
+        <v>-4.9849648172519103</v>
+      </c>
+      <c r="D115">
+        <v>-4.9849648172519103</v>
+      </c>
+      <c r="E115">
+        <f>AVERAGE(C115,D115)</f>
+        <v>-4.9849648172519103</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A116" t="s">
+        <v>439</v>
+      </c>
+      <c r="B116" s="7">
+        <v>43559</v>
+      </c>
+      <c r="C116">
+        <v>-24.118994808956501</v>
+      </c>
+      <c r="D116">
+        <v>-24.118994808956501</v>
+      </c>
+      <c r="E116">
+        <f>AVERAGE(C116,D116)</f>
+        <v>-24.118994808956501</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A117" t="s">
+        <v>440</v>
+      </c>
+      <c r="B117" s="7">
+        <v>45288</v>
+      </c>
+      <c r="C117">
+        <v>-18.4534747941013</v>
+      </c>
+      <c r="D117">
+        <v>-18.4534747941013</v>
+      </c>
+      <c r="E117">
+        <f>AVERAGE(C117,D117)</f>
+        <v>-18.4534747941013</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A118" t="s">
+        <v>441</v>
+      </c>
+      <c r="B118" s="7">
+        <v>44970</v>
+      </c>
+      <c r="C118">
+        <v>-22.414204897113901</v>
+      </c>
+      <c r="D118">
+        <v>-22.414204897113901</v>
+      </c>
+      <c r="E118">
+        <f>AVERAGE(C118,D118)</f>
+        <v>-22.414204897113901</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A119" t="s">
+        <v>442</v>
+      </c>
+      <c r="B119" s="7">
+        <v>40890</v>
+      </c>
+      <c r="C119">
+        <v>-4.5049495695152002</v>
+      </c>
+      <c r="D119">
+        <v>-4.5049495695152002</v>
+      </c>
+      <c r="E119">
+        <f>AVERAGE(C119,D119)</f>
+        <v>-4.5049495695152002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A120" t="s">
+        <v>443</v>
+      </c>
+      <c r="B120" s="7">
+        <v>39031</v>
+      </c>
+      <c r="C120">
+        <v>-25.398161015393701</v>
+      </c>
+      <c r="D120">
+        <v>-25.398161015393701</v>
+      </c>
+      <c r="E120">
+        <f>AVERAGE(C120,D120)</f>
+        <v>-25.398161015393701</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A121" t="s">
+        <v>444</v>
+      </c>
+      <c r="B121" s="7">
+        <v>39031</v>
+      </c>
+      <c r="C121">
+        <v>-22.592099411718799</v>
+      </c>
+      <c r="D121">
+        <v>-22.592099411718799</v>
+      </c>
+      <c r="E121">
+        <f>AVERAGE(C121,D121)</f>
+        <v>-22.592099411718799</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A122" t="s">
+        <v>445</v>
+      </c>
+      <c r="B122" s="7">
+        <v>36853</v>
+      </c>
+      <c r="C122">
+        <v>-15.387194650779</v>
+      </c>
+      <c r="D122">
+        <v>-12.6038763691979</v>
+      </c>
+      <c r="E122">
+        <f>AVERAGE(C122,D122)</f>
+        <v>-13.99553550998845</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A123" t="s">
+        <v>446</v>
+      </c>
+      <c r="B123" s="7">
+        <v>42038</v>
+      </c>
+      <c r="C123">
+        <v>-23.379175275965899</v>
+      </c>
+      <c r="D123">
+        <v>-21.4105789336278</v>
+      </c>
+      <c r="E123">
+        <f>AVERAGE(C123,D123)</f>
+        <v>-22.394877104796848</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A124" t="s">
+        <v>447</v>
+      </c>
+      <c r="B124" s="7">
+        <v>38714</v>
+      </c>
+      <c r="C124">
+        <v>-29.5719118358648</v>
+      </c>
+      <c r="D124">
+        <v>-29.5719118358648</v>
+      </c>
+      <c r="E124">
+        <f>AVERAGE(C124,D124)</f>
+        <v>-29.5719118358648</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A125" t="s">
+        <v>448</v>
+      </c>
+      <c r="B125" s="7">
+        <v>39031</v>
+      </c>
+      <c r="C125">
+        <v>-39.740898437356499</v>
+      </c>
+      <c r="D125">
+        <v>-39.740898437356499</v>
+      </c>
+      <c r="E125">
+        <f>AVERAGE(C125,D125)</f>
+        <v>-39.740898437356499</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A126" t="s">
+        <v>449</v>
+      </c>
+      <c r="B126" s="7">
+        <v>40493</v>
+      </c>
+      <c r="C126">
+        <v>-26.503239007801099</v>
+      </c>
+      <c r="D126">
+        <v>-26.503239007801099</v>
+      </c>
+      <c r="E126">
+        <f>AVERAGE(C126,D126)</f>
+        <v>-26.503239007801099</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A127" t="s">
+        <v>450</v>
+      </c>
+      <c r="B127" s="7">
+        <v>36853</v>
+      </c>
+      <c r="C127">
+        <v>-24.2006452422198</v>
+      </c>
+      <c r="D127">
+        <v>-24.2006452422198</v>
+      </c>
+      <c r="E127">
+        <f>AVERAGE(C127,D127)</f>
+        <v>-24.2006452422198</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A128" t="s">
+        <v>451</v>
+      </c>
+      <c r="B128" s="7">
+        <v>40807</v>
+      </c>
+      <c r="C128">
+        <v>-16.285992446368802</v>
+      </c>
+      <c r="D128">
+        <v>-15.6156106274642</v>
+      </c>
+      <c r="E128">
+        <f>AVERAGE(C128,D128)</f>
+        <v>-15.950801536916501</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A129" t="s">
+        <v>452</v>
+      </c>
+      <c r="B129" s="7">
+        <v>44391</v>
+      </c>
+      <c r="C129">
+        <v>-11.206895093754101</v>
+      </c>
+      <c r="D129">
+        <v>-11.206895093754101</v>
+      </c>
+      <c r="E129">
+        <f>AVERAGE(C129,D129)</f>
+        <v>-11.206895093754101</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A130" t="s">
+        <v>453</v>
+      </c>
+      <c r="B130" s="7">
+        <v>44592</v>
+      </c>
+      <c r="C130">
+        <v>-6.8736110399203403</v>
+      </c>
+      <c r="D130">
+        <v>-6.8736110399203403</v>
+      </c>
+      <c r="E130">
+        <f>AVERAGE(C130,D130)</f>
+        <v>-6.8736110399203403</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A131" t="s">
+        <v>454</v>
+      </c>
+      <c r="B131" s="7">
+        <v>45313</v>
+      </c>
+      <c r="C131">
+        <v>-8.1880671918709993</v>
+      </c>
+      <c r="D131">
+        <v>-8.1880671918709993</v>
+      </c>
+      <c r="E131">
+        <f>AVERAGE(C131,D131)</f>
+        <v>-8.1880671918709993</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A132" t="s">
+        <v>455</v>
+      </c>
+      <c r="B132" s="7">
+        <v>44389</v>
+      </c>
+      <c r="C132">
+        <v>-11.776401685631701</v>
+      </c>
+      <c r="D132">
+        <v>-11.776401685631701</v>
+      </c>
+      <c r="E132">
+        <f>AVERAGE(C132,D132)</f>
+        <v>-11.776401685631701</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A133" t="s">
+        <v>456</v>
+      </c>
+      <c r="B133" s="7">
+        <v>44383</v>
+      </c>
+      <c r="C133">
+        <v>-8.0810489076610406</v>
+      </c>
+      <c r="D133">
+        <v>-8.0810489076610406</v>
+      </c>
+      <c r="E133">
+        <f>AVERAGE(C133,D133)</f>
+        <v>-8.0810489076610406</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A134" t="s">
+        <v>457</v>
+      </c>
+      <c r="B134" s="7">
+        <v>40932</v>
+      </c>
+      <c r="C134">
+        <v>-40.249675471561702</v>
+      </c>
+      <c r="D134">
+        <v>-38.173720967733402</v>
+      </c>
+      <c r="E134">
+        <f>AVERAGE(C134,D134)</f>
+        <v>-39.211698219647552</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A135" t="s">
+        <v>458</v>
+      </c>
+      <c r="B135" s="7">
+        <v>40205</v>
+      </c>
+      <c r="C135">
+        <v>-30.349012954341099</v>
+      </c>
+      <c r="D135">
+        <v>-30.349012954341099</v>
+      </c>
+      <c r="E135">
+        <f>AVERAGE(C135,D135)</f>
+        <v>-30.349012954341099</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A136" t="s">
+        <v>459</v>
+      </c>
+      <c r="B136" s="7">
+        <v>40205</v>
+      </c>
+      <c r="C136">
+        <v>-37.752807274293303</v>
+      </c>
+      <c r="D136">
+        <v>-31.6724219600843</v>
+      </c>
+      <c r="E136">
+        <f>AVERAGE(C136,D136)</f>
+        <v>-34.712614617188805</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A137" t="s">
+        <v>460</v>
+      </c>
+      <c r="B137" s="7">
+        <v>44095</v>
+      </c>
+      <c r="C137">
+        <v>-16.717469667120401</v>
+      </c>
+      <c r="D137">
+        <v>-16.717469667120401</v>
+      </c>
+      <c r="E137">
+        <f>AVERAGE(C137,D137)</f>
+        <v>-16.717469667120401</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A138" t="s">
+        <v>461</v>
+      </c>
+      <c r="B138" s="7">
+        <v>44088</v>
+      </c>
+      <c r="C138">
+        <v>-23.483029616293301</v>
+      </c>
+      <c r="D138">
+        <v>-23.483029616293301</v>
+      </c>
+      <c r="E138">
+        <f>AVERAGE(C138,D138)</f>
+        <v>-23.483029616293301</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A139" t="s">
+        <v>462</v>
+      </c>
+      <c r="B139" s="7">
+        <v>44084</v>
+      </c>
+      <c r="C139">
+        <v>-24.927758434220301</v>
+      </c>
+      <c r="D139">
+        <v>-24.927758434220301</v>
+      </c>
+      <c r="E139">
+        <f>AVERAGE(C139,D139)</f>
+        <v>-24.927758434220301</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A140" t="s">
+        <v>463</v>
+      </c>
+      <c r="B140" s="7">
+        <v>44085</v>
+      </c>
+      <c r="C140">
+        <v>-20.379367494364299</v>
+      </c>
+      <c r="D140">
+        <v>-20.379367494364299</v>
+      </c>
+      <c r="E140">
+        <f>AVERAGE(C140,D140)</f>
+        <v>-20.379367494364299</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A141" t="s">
+        <v>464</v>
+      </c>
+      <c r="B141" s="7">
+        <v>39254</v>
+      </c>
+      <c r="C141">
+        <v>-50.073420701587601</v>
+      </c>
+      <c r="D141">
+        <v>-25.852785480296902</v>
+      </c>
+      <c r="E141">
+        <f>AVERAGE(C141,D141)</f>
+        <v>-37.963103090942255</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A142" t="s">
+        <v>465</v>
+      </c>
+      <c r="B142" s="7">
+        <v>39254</v>
+      </c>
+      <c r="C142">
+        <v>-32.7957014604048</v>
+      </c>
+      <c r="D142">
+        <v>-20.928339715798199</v>
+      </c>
+      <c r="E142">
+        <f>AVERAGE(C142,D142)</f>
+        <v>-26.862020588101501</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A143" t="s">
+        <v>466</v>
+      </c>
+      <c r="B143" s="7">
+        <v>40493</v>
+      </c>
+      <c r="C143">
+        <v>-45.338445398330002</v>
+      </c>
+      <c r="D143">
+        <v>-45.338445398330002</v>
+      </c>
+      <c r="E143">
+        <f>AVERAGE(C143,D143)</f>
+        <v>-45.338445398330002</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A144" t="s">
+        <v>467</v>
+      </c>
+      <c r="B144" s="7">
+        <v>38714</v>
+      </c>
+      <c r="C144">
+        <v>-56.958128881569003</v>
+      </c>
+      <c r="D144">
+        <v>-27.0761245746105</v>
+      </c>
+      <c r="E144">
+        <f>AVERAGE(C144,D144)</f>
+        <v>-42.01712672808975</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A145" t="s">
+        <v>468</v>
+      </c>
+      <c r="B145" s="7">
+        <v>43700</v>
+      </c>
+      <c r="C145">
+        <v>-17.8236192605269</v>
+      </c>
+      <c r="D145">
+        <v>-17.8236192605269</v>
+      </c>
+      <c r="E145">
+        <f>AVERAGE(C145,D145)</f>
+        <v>-17.8236192605269</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A146" t="s">
+        <v>469</v>
+      </c>
+      <c r="B146" s="7">
+        <v>43691</v>
+      </c>
+      <c r="C146">
+        <v>-29.742906598210102</v>
+      </c>
+      <c r="D146">
+        <v>-29.742906598210102</v>
+      </c>
+      <c r="E146">
+        <f>AVERAGE(C146,D146)</f>
+        <v>-29.742906598210102</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A147" t="s">
+        <v>470</v>
+      </c>
+      <c r="B147" s="7">
+        <v>43691</v>
+      </c>
+      <c r="C147">
+        <v>-17.670435824222501</v>
+      </c>
+      <c r="D147">
+        <v>-17.670435824222501</v>
+      </c>
+      <c r="E147">
+        <f>AVERAGE(C147,D147)</f>
+        <v>-17.670435824222501</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A148" t="s">
+        <v>471</v>
+      </c>
+      <c r="B148" s="7">
+        <v>39841</v>
+      </c>
+      <c r="C148">
+        <v>-33.708529995714102</v>
+      </c>
+      <c r="D148">
+        <v>-33.708529995714102</v>
+      </c>
+      <c r="E148">
+        <f>AVERAGE(C148,D148)</f>
+        <v>-33.708529995714102</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A149" t="s">
+        <v>472</v>
+      </c>
+      <c r="B149" s="7">
+        <v>37551</v>
+      </c>
+      <c r="C149">
+        <v>-62.043797358178999</v>
+      </c>
+      <c r="D149">
+        <v>-46.735554955037998</v>
+      </c>
+      <c r="E149">
+        <f>AVERAGE(C149,D149)</f>
+        <v>-54.389676156608502</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B149">
+    <sortCondition ref="B4:B149"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A99BE8-174B-D442-B404-558060C3B728}">
+  <dimension ref="A1:C146"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B146"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1">_xlfn.TEXTJOIN(", ", TRUE, IF(all!E2:E170&lt;&gt;"", CHAR(34) &amp; all!E2:E170 &amp; ".TO" &amp; CHAR(34), ""))</f>
-        <v>"SVR.TO", "IBIT.TO", "CGL.TO", "XMV.TO", "XMI.TO", "XML.TO", "XIN.TO", "XMS.TO", "XMY.TO", "XEM.TO", "XMM.TO", "XEC.TO", "XUS.TO", "XEF.TO", "XMH.TO", "XMC.TO", "XDIV.TO", "XMU.TO", "XQQ.TO", "XWD.TO", "XDUH.TO", "XDG.TO", "XSU.TO", "XDU.TO", "XSUS.TO", "XSEA.TO", "XDGH.TO", "XESG.TO", "XGI.TO", "XCD.TO", "XSEM.TO", "XSP.TO", "CWO.TO", "CRQ.TO", "XID.TO", "XCH.TO", "XEMC.TO", "XHC.TO", "XDRV.TO", "CWW.TO", "XCV.TO", "XCG.TO", "XUSR.TO", "XDV.TO", "XDSR.TO", "XEU.TO", "CEW.TO", "XEH.TO", "XUU.TO", "COW.TO", "CIF.TO", "CYH.TO", "XDNA.TO", "XCLN.TO", "XQQU.TO", "XEXP.TO", "XAW.TO", "XHAK.TO", "XETM.TO", "XCHP.TO", "CIE.TO", "XUSF.TO", "XAD.TO", "XEN.TO", "CUD.TO", "CDZ.TO", "XQLT.TO", "XIU.TO", "CJP.TO", "XEG.TO", "XST.TO", "XIC.TO", "CPD.TO", "XSMC.TO", "XMA.TO", "XUSC.TO", "XSMH.TO", "XFH.TO", "XIT.TO", "XFN.TO", "XMTM.TO", "XBM.TO", "XEI.TO", "XVLU.TO", "XMD.TO", "XUT.TO", "XCSR.TO", "XPF.TO", "XHU.TO", "XGD.TO", "XSPC.TO", "XUH.TO", "XCS.TO", "XHD.TO", "CLU.TO", "XMW.TO", "XSC.TO", "XSE.TO", "CMR.TO", "CLG.TO", "CBH.TO", "CLF.TO", "CBO.TO", "XGGB.TO", "CVD.TO", "XQB.TO", "XAGG.TO", "XCBG.TO", "XSHG.TO", "XAGH.TO", "XSTB.TO", "XFLB.TO", "XFLI.TO", "XFLX.TO", "XSAB.TO", "XTLH.TO", "XTLT.TO", "XFR.TO", "XGB.TO", "XCB.TO", "XSB.TO", "XSI.TO", "XRB.TO", "XLB.TO", "XHB.TO", "XBB.TO", "XSH.TO", "XSTH.TO", "XSTP.TO", "XCBU.TO", "XIGS.TO", "XSHU.TO", "XEB.TO", "XIG.TO", "XHY.TO", "GCNS.TO", "GGRO.TO", "GEQT.TO", "GBAL.TO", "XGRO.TO", "XBAL.TO", "FIE.TO", "XTR.TO", "XCNS.TO", "XEQT.TO", "XINC.TO", "CGR.TO", "XRE.TO"</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
-        <v>326</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1" s="7">
+        <v>40115</v>
+      </c>
+      <c r="C1" s="7">
+        <f>AVERAGE(B1:B146)</f>
+        <v>41598.773972602743</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" s="7">
+        <v>40455</v>
+      </c>
+      <c r="C2" s="7">
+        <f>MIN(B1:B146)</f>
+        <v>36437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3" s="7">
+        <v>41124</v>
+      </c>
+      <c r="C3" s="7">
+        <f>MAX(B1:B146)</f>
+        <v>45569</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B4" s="7">
+        <v>41138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" s="7">
+        <v>42471</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>332</v>
+      </c>
+      <c r="B6" s="7">
+        <v>37361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>333</v>
+      </c>
+      <c r="B7" s="7">
+        <v>42471</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>334</v>
+      </c>
+      <c r="B8" s="7">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>335</v>
+      </c>
+      <c r="B9" s="7">
+        <v>40115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>336</v>
+      </c>
+      <c r="B10" s="7">
+        <v>41137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>337</v>
+      </c>
+      <c r="B11" s="7">
+        <v>41379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>338</v>
+      </c>
+      <c r="B12" s="7">
+        <v>41379</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>339</v>
+      </c>
+      <c r="B13" s="7">
+        <v>41379</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>340</v>
+      </c>
+      <c r="B14" s="7">
+        <v>42227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>341</v>
+      </c>
+      <c r="B15" s="7">
+        <v>42226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>342</v>
+      </c>
+      <c r="B16" s="7">
+        <v>42901</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>343</v>
+      </c>
+      <c r="B17" s="7">
+        <v>41124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>344</v>
+      </c>
+      <c r="B18" s="7">
+        <v>40673</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>345</v>
+      </c>
+      <c r="B19" s="7">
+        <v>40115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>346</v>
+      </c>
+      <c r="B20" s="7">
+        <v>43109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>347</v>
+      </c>
+      <c r="B21" s="7">
+        <v>43109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>348</v>
+      </c>
+      <c r="B22" s="7">
+        <v>39220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>349</v>
+      </c>
+      <c r="B23" s="7">
+        <v>42901</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>350</v>
+      </c>
+      <c r="B24" s="7">
+        <v>43546</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>351</v>
+      </c>
+      <c r="B25" s="7">
+        <v>43550</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>352</v>
+      </c>
+      <c r="B26" s="7">
+        <v>43011</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>353</v>
+      </c>
+      <c r="B27" s="7">
+        <v>43559</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>354</v>
+      </c>
+      <c r="B28" s="7">
+        <v>41372</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>355</v>
+      </c>
+      <c r="B29" s="7">
+        <v>41372</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>356</v>
+      </c>
+      <c r="B30" s="7">
+        <v>43546</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>357</v>
+      </c>
+      <c r="B31" s="7">
+        <v>37361</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>358</v>
+      </c>
+      <c r="B32" s="7">
+        <v>39910</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>359</v>
+      </c>
+      <c r="B33" s="7">
+        <v>39815</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>360</v>
+      </c>
+      <c r="B34" s="7">
+        <v>40205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>361</v>
+      </c>
+      <c r="B35" s="7">
+        <v>40205</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>362</v>
+      </c>
+      <c r="B36" s="7">
+        <v>44972</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>363</v>
+      </c>
+      <c r="B37" s="7">
+        <v>40932</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>364</v>
+      </c>
+      <c r="B38" s="7">
+        <v>44978</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>365</v>
+      </c>
+      <c r="B39" s="7">
+        <v>39380</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>366</v>
+      </c>
+      <c r="B40" s="7">
+        <v>39031</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>367</v>
+      </c>
+      <c r="B41" s="7">
+        <v>39031</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>368</v>
+      </c>
+      <c r="B42" s="7">
+        <v>43944</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>369</v>
+      </c>
+      <c r="B43" s="7">
+        <v>38714</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>370</v>
+      </c>
+      <c r="B44" s="7">
+        <v>43956</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>371</v>
+      </c>
+      <c r="B45" s="7">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>372</v>
+      </c>
+      <c r="B46" s="7">
+        <v>39491</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>373</v>
+      </c>
+      <c r="B47" s="7">
+        <v>41753</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>374</v>
+      </c>
+      <c r="B48" s="7">
+        <v>42055</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>375</v>
+      </c>
+      <c r="B49" s="7">
+        <v>39435</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>376</v>
+      </c>
+      <c r="B50" s="7">
+        <v>39841</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>377</v>
+      </c>
+      <c r="B51" s="7">
+        <v>39464</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>378</v>
+      </c>
+      <c r="B52" s="7">
+        <v>44685</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>379</v>
+      </c>
+      <c r="B53" s="7">
+        <v>44685</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>380</v>
+      </c>
+      <c r="B54" s="7">
+        <v>45182</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
+        <v>381</v>
+      </c>
+      <c r="B55" s="7">
+        <v>44712</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>382</v>
+      </c>
+      <c r="B56" s="7">
+        <v>42055</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>383</v>
+      </c>
+      <c r="B57" s="7">
+        <v>44685</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>384</v>
+      </c>
+      <c r="B58" s="7">
+        <v>45182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>385</v>
+      </c>
+      <c r="B59" s="7">
+        <v>45183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>386</v>
+      </c>
+      <c r="B60" s="7">
+        <v>39815</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>387</v>
+      </c>
+      <c r="B61" s="7">
+        <v>45175</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>388</v>
+      </c>
+      <c r="B62" s="7">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>389</v>
+      </c>
+      <c r="B63" s="7">
+        <v>39220</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
+        <v>390</v>
+      </c>
+      <c r="B64" s="7">
+        <v>40813</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>391</v>
+      </c>
+      <c r="B65" s="7">
+        <v>38968</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>392</v>
+      </c>
+      <c r="B66" s="7">
+        <v>43720</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>393</v>
+      </c>
+      <c r="B67" s="7">
+        <v>36437</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>394</v>
+      </c>
+      <c r="B68" s="7">
+        <v>39815</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A69" t="s">
+        <v>395</v>
+      </c>
+      <c r="B69" s="7">
+        <v>36973</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>396</v>
+      </c>
+      <c r="B70" s="7">
+        <v>40932</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>397</v>
+      </c>
+      <c r="B71" s="7">
+        <v>36944</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>398</v>
+      </c>
+      <c r="B72" s="7">
+        <v>39380</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>399</v>
+      </c>
+      <c r="B73" s="7">
+        <v>43720</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>400</v>
+      </c>
+      <c r="B74" s="7">
+        <v>38714</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>401</v>
+      </c>
+      <c r="B75" s="7">
+        <v>45491</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
+        <v>402</v>
+      </c>
+      <c r="B76" s="7">
+        <v>43720</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A77" t="s">
+        <v>403</v>
+      </c>
+      <c r="B77" s="7">
+        <v>42055</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A78" t="s">
+        <v>404</v>
+      </c>
+      <c r="B78" s="7">
+        <v>36973</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A79" t="s">
+        <v>405</v>
+      </c>
+      <c r="B79" s="7">
+        <v>36979</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A80" t="s">
+        <v>406</v>
+      </c>
+      <c r="B80" s="7">
+        <v>43725</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A81" t="s">
+        <v>407</v>
+      </c>
+      <c r="B81" s="7">
+        <v>40932</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A82" t="s">
+        <v>408</v>
+      </c>
+      <c r="B82" s="7">
+        <v>40932</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A83" t="s">
+        <v>409</v>
+      </c>
+      <c r="B83" s="7">
+        <v>43720</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A84" t="s">
+        <v>410</v>
+      </c>
+      <c r="B84" s="7">
+        <v>36958</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A85" t="s">
+        <v>411</v>
+      </c>
+      <c r="B85" s="7">
+        <v>40932</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A86" t="s">
+        <v>412</v>
+      </c>
+      <c r="B86" s="7">
+        <v>43944</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A87" t="s">
+        <v>413</v>
+      </c>
+      <c r="B87" s="7">
+        <v>40504</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A88" t="s">
+        <v>414</v>
+      </c>
+      <c r="B88" s="7">
+        <v>42055</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A89" t="s">
+        <v>415</v>
+      </c>
+      <c r="B89" s="7">
+        <v>36979</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A90" t="s">
+        <v>416</v>
+      </c>
+      <c r="B90" s="7">
+        <v>45492</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A91" t="s">
+        <v>417</v>
+      </c>
+      <c r="B91" s="7">
+        <v>42055</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A92" t="s">
+        <v>418</v>
+      </c>
+      <c r="B92" s="7">
+        <v>39220</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A93" t="s">
+        <v>419</v>
+      </c>
+      <c r="B93" s="7">
+        <v>41141</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A94" t="s">
+        <v>420</v>
+      </c>
+      <c r="B94" s="7">
+        <v>39815</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A95" t="s">
+        <v>421</v>
+      </c>
+      <c r="B95" s="7">
+        <v>41134</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A96" t="s">
+        <v>422</v>
+      </c>
+      <c r="B96" s="7">
+        <v>42269</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A97" t="s">
+        <v>423</v>
+      </c>
+      <c r="B97" s="7">
+        <v>42640</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A98" t="s">
+        <v>424</v>
+      </c>
+      <c r="B98" s="7">
+        <v>39497</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A99" t="s">
+        <v>425</v>
+      </c>
+      <c r="B99" s="7">
+        <v>40952</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A100" t="s">
+        <v>426</v>
+      </c>
+      <c r="B100" s="7">
+        <v>40952</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A101" t="s">
+        <v>427</v>
+      </c>
+      <c r="B101" s="7">
+        <v>39491</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A102" t="s">
+        <v>428</v>
+      </c>
+      <c r="B102" s="7">
+        <v>40151</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A103" t="s">
+        <v>429</v>
+      </c>
+      <c r="B103" s="7">
+        <v>40708</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A104" t="s">
+        <v>430</v>
+      </c>
+      <c r="B104" s="7">
+        <v>40288</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A105" t="s">
+        <v>431</v>
+      </c>
+      <c r="B105" s="7">
+        <v>45309</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A106" t="s">
+        <v>432</v>
+      </c>
+      <c r="B106" s="7">
+        <v>44404</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A107" t="s">
+        <v>433</v>
+      </c>
+      <c r="B107" s="7">
+        <v>44404</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A108" t="s">
+        <v>434</v>
+      </c>
+      <c r="B108" s="7">
+        <v>44404</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A109" t="s">
+        <v>435</v>
+      </c>
+      <c r="B109" s="7">
+        <v>43565</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A110" t="s">
+        <v>436</v>
+      </c>
+      <c r="B110" s="7">
+        <v>44964</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A111" t="s">
+        <v>437</v>
+      </c>
+      <c r="B111" s="7">
+        <v>45561</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A112" t="s">
+        <v>438</v>
+      </c>
+      <c r="B112" s="7">
+        <v>45569</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A113" t="s">
+        <v>439</v>
+      </c>
+      <c r="B113" s="7">
+        <v>43559</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A114" t="s">
+        <v>440</v>
+      </c>
+      <c r="B114" s="7">
+        <v>45288</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A115" t="s">
+        <v>441</v>
+      </c>
+      <c r="B115" s="7">
+        <v>44970</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A116" t="s">
+        <v>442</v>
+      </c>
+      <c r="B116" s="7">
+        <v>40890</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A117" t="s">
+        <v>443</v>
+      </c>
+      <c r="B117" s="7">
+        <v>39031</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A118" t="s">
+        <v>444</v>
+      </c>
+      <c r="B118" s="7">
+        <v>39031</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A119" t="s">
+        <v>445</v>
+      </c>
+      <c r="B119" s="7">
+        <v>36853</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A120" t="s">
+        <v>446</v>
+      </c>
+      <c r="B120" s="7">
+        <v>42038</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A121" t="s">
+        <v>447</v>
+      </c>
+      <c r="B121" s="7">
+        <v>38714</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A122" t="s">
+        <v>448</v>
+      </c>
+      <c r="B122" s="7">
+        <v>39031</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A123" t="s">
+        <v>449</v>
+      </c>
+      <c r="B123" s="7">
+        <v>40493</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A124" t="s">
+        <v>450</v>
+      </c>
+      <c r="B124" s="7">
+        <v>36853</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A125" t="s">
+        <v>451</v>
+      </c>
+      <c r="B125" s="7">
+        <v>40807</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A126" t="s">
+        <v>452</v>
+      </c>
+      <c r="B126" s="7">
+        <v>44391</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A127" t="s">
+        <v>453</v>
+      </c>
+      <c r="B127" s="7">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A128" t="s">
+        <v>454</v>
+      </c>
+      <c r="B128" s="7">
+        <v>45313</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A129" t="s">
+        <v>455</v>
+      </c>
+      <c r="B129" s="7">
+        <v>44389</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A130" t="s">
+        <v>456</v>
+      </c>
+      <c r="B130" s="7">
+        <v>44383</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A131" t="s">
+        <v>457</v>
+      </c>
+      <c r="B131" s="7">
+        <v>40932</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A132" t="s">
+        <v>458</v>
+      </c>
+      <c r="B132" s="7">
+        <v>40205</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A133" t="s">
+        <v>459</v>
+      </c>
+      <c r="B133" s="7">
+        <v>40205</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A134" t="s">
+        <v>460</v>
+      </c>
+      <c r="B134" s="7">
+        <v>44095</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A135" t="s">
+        <v>461</v>
+      </c>
+      <c r="B135" s="7">
+        <v>44088</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A136" t="s">
+        <v>462</v>
+      </c>
+      <c r="B136" s="7">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A137" t="s">
+        <v>463</v>
+      </c>
+      <c r="B137" s="7">
+        <v>44085</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A138" t="s">
+        <v>464</v>
+      </c>
+      <c r="B138" s="7">
+        <v>39254</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A139" t="s">
+        <v>465</v>
+      </c>
+      <c r="B139" s="7">
+        <v>39254</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A140" t="s">
+        <v>466</v>
+      </c>
+      <c r="B140" s="7">
+        <v>40493</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A141" t="s">
+        <v>467</v>
+      </c>
+      <c r="B141" s="7">
+        <v>38714</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A142" t="s">
+        <v>468</v>
+      </c>
+      <c r="B142" s="7">
+        <v>43700</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A143" t="s">
+        <v>469</v>
+      </c>
+      <c r="B143" s="7">
+        <v>43691</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A144" t="s">
+        <v>470</v>
+      </c>
+      <c r="B144" s="7">
+        <v>43691</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A145" t="s">
+        <v>471</v>
+      </c>
+      <c r="B145" s="7">
+        <v>39841</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A146" t="s">
+        <v>472</v>
+      </c>
+      <c r="B146" s="7">
+        <v>37551</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>